<commit_message>
- Resolved PA ballot comments
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@1389 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/ballots/2013-01 Draft/Comments-FHIR_R1_O2_2013JAN.xlsx
+++ b/ballots/2013-01 Draft/Comments-FHIR_R1_O2_2013JAN.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11255" uniqueCount="2554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11265" uniqueCount="2554">
   <si>
     <t xml:space="preserve">BALLOT TITLE: </t>
   </si>
@@ -12409,23 +12409,12 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="42" fillId="37" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="11" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="10" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -12433,14 +12422,14 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -12453,6 +12442,12 @@
     <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -12478,23 +12473,32 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="11" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="10" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="28" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -12510,114 +12514,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="36" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="22" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="42" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -12661,6 +12557,114 @@
     <xf numFmtId="0" fontId="23" fillId="36" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="22" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="42" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="36" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -12677,9 +12681,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12700,9 +12701,8 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="37" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="56">
@@ -13095,20 +13095,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:99" ht="45.75" customHeight="1" thickTop="1">
-      <c r="A1" s="249" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="249"/>
-      <c r="C1" s="249"/>
-      <c r="D1" s="250"/>
+      <c r="A1" s="246" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="247"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="251" t="s">
+      <c r="F1" s="268" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="252"/>
-      <c r="H1" s="252"/>
-      <c r="I1" s="252"/>
-      <c r="J1" s="253"/>
+      <c r="G1" s="269"/>
+      <c r="H1" s="269"/>
+      <c r="I1" s="269"/>
+      <c r="J1" s="270"/>
       <c r="K1" s="4"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -13116,12 +13116,12 @@
       <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:99">
-      <c r="A2" s="249" t="s">
+      <c r="A2" s="246" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="249"/>
-      <c r="C2" s="249"/>
-      <c r="D2" s="250"/>
+      <c r="B2" s="246"/>
+      <c r="C2" s="246"/>
+      <c r="D2" s="247"/>
       <c r="E2" s="3"/>
       <c r="F2" s="6" t="s">
         <v>3</v>
@@ -13137,20 +13137,20 @@
       <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:99" ht="18.75" customHeight="1">
-      <c r="A3" s="244" t="s">
+      <c r="A3" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="244"/>
-      <c r="C3" s="244"/>
-      <c r="D3" s="245"/>
+      <c r="B3" s="263"/>
+      <c r="C3" s="263"/>
+      <c r="D3" s="264"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="254" t="s">
+      <c r="F3" s="251" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="255"/>
-      <c r="H3" s="255"/>
-      <c r="I3" s="255"/>
-      <c r="J3" s="256"/>
+      <c r="G3" s="252"/>
+      <c r="H3" s="252"/>
+      <c r="I3" s="252"/>
+      <c r="J3" s="253"/>
       <c r="K3" s="10"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -13158,18 +13158,18 @@
       <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:99" ht="18.75" customHeight="1">
-      <c r="A4" s="244" t="s">
+      <c r="A4" s="263" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="244"/>
-      <c r="C4" s="244"/>
-      <c r="D4" s="245"/>
+      <c r="B4" s="263"/>
+      <c r="C4" s="263"/>
+      <c r="D4" s="264"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="246"/>
-      <c r="G4" s="247"/>
-      <c r="H4" s="247"/>
-      <c r="I4" s="247"/>
-      <c r="J4" s="248"/>
+      <c r="F4" s="265"/>
+      <c r="G4" s="266"/>
+      <c r="H4" s="266"/>
+      <c r="I4" s="266"/>
+      <c r="J4" s="267"/>
       <c r="K4" s="10"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
@@ -13177,18 +13177,18 @@
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:99" ht="18.75" customHeight="1">
-      <c r="A5" s="257" t="s">
+      <c r="A5" s="256" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="257"/>
-      <c r="C5" s="257"/>
-      <c r="D5" s="258"/>
+      <c r="B5" s="256"/>
+      <c r="C5" s="256"/>
+      <c r="D5" s="257"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="254"/>
-      <c r="G5" s="255"/>
-      <c r="H5" s="255"/>
-      <c r="I5" s="255"/>
-      <c r="J5" s="256"/>
+      <c r="F5" s="251"/>
+      <c r="G5" s="252"/>
+      <c r="H5" s="252"/>
+      <c r="I5" s="252"/>
+      <c r="J5" s="253"/>
       <c r="K5" s="10"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -13196,18 +13196,18 @@
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:99" ht="29.25" customHeight="1">
-      <c r="A6" s="259" t="s">
+      <c r="A6" s="258" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="259"/>
-      <c r="C6" s="259"/>
-      <c r="D6" s="260"/>
+      <c r="B6" s="258"/>
+      <c r="C6" s="258"/>
+      <c r="D6" s="259"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="254"/>
-      <c r="G6" s="255"/>
-      <c r="H6" s="255"/>
-      <c r="I6" s="255"/>
-      <c r="J6" s="256"/>
+      <c r="F6" s="251"/>
+      <c r="G6" s="252"/>
+      <c r="H6" s="252"/>
+      <c r="I6" s="252"/>
+      <c r="J6" s="253"/>
       <c r="K6" s="10"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
@@ -13215,18 +13215,18 @@
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:99" ht="15.75" customHeight="1">
-      <c r="A7" s="249" t="s">
+      <c r="A7" s="246" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="249"/>
-      <c r="C7" s="249"/>
-      <c r="D7" s="250"/>
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="247"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="261"/>
-      <c r="G7" s="262"/>
-      <c r="H7" s="262"/>
-      <c r="I7" s="262"/>
-      <c r="J7" s="263"/>
+      <c r="F7" s="260"/>
+      <c r="G7" s="261"/>
+      <c r="H7" s="261"/>
+      <c r="I7" s="261"/>
+      <c r="J7" s="262"/>
       <c r="K7" s="4"/>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
@@ -13236,18 +13236,18 @@
       <c r="CU7" s="16"/>
     </row>
     <row r="8" spans="1:99" ht="17.25" customHeight="1">
-      <c r="A8" s="249" t="s">
+      <c r="A8" s="246" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="249"/>
-      <c r="C8" s="249"/>
-      <c r="D8" s="250"/>
+      <c r="B8" s="246"/>
+      <c r="C8" s="246"/>
+      <c r="D8" s="247"/>
       <c r="E8" s="17"/>
-      <c r="F8" s="265"/>
-      <c r="G8" s="266"/>
-      <c r="H8" s="266"/>
-      <c r="I8" s="266"/>
-      <c r="J8" s="267"/>
+      <c r="F8" s="248"/>
+      <c r="G8" s="249"/>
+      <c r="H8" s="249"/>
+      <c r="I8" s="249"/>
+      <c r="J8" s="250"/>
       <c r="K8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
@@ -13255,18 +13255,18 @@
       <c r="P8" s="10"/>
     </row>
     <row r="9" spans="1:99" ht="62.25" customHeight="1">
-      <c r="A9" s="249" t="s">
+      <c r="A9" s="246" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="249"/>
-      <c r="C9" s="249"/>
-      <c r="D9" s="250"/>
+      <c r="B9" s="246"/>
+      <c r="C9" s="246"/>
+      <c r="D9" s="247"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="254"/>
-      <c r="G9" s="255"/>
-      <c r="H9" s="255"/>
-      <c r="I9" s="255"/>
-      <c r="J9" s="256"/>
+      <c r="F9" s="251"/>
+      <c r="G9" s="252"/>
+      <c r="H9" s="252"/>
+      <c r="I9" s="252"/>
+      <c r="J9" s="253"/>
       <c r="K9" s="18"/>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
@@ -13274,19 +13274,19 @@
       <c r="P9" s="19"/>
     </row>
     <row r="10" spans="1:99" ht="66.75" customHeight="1">
-      <c r="A10" s="268">
+      <c r="A10" s="254">
         <f>IF(Ov=Setup!C9,Disclaimer2,IF(Ov=Setup!B9,Disclaimer,IF(Ov=Setup!D9,,)))</f>
         <v>0</v>
       </c>
-      <c r="B10" s="268"/>
-      <c r="C10" s="268"/>
-      <c r="D10" s="268"/>
-      <c r="E10" s="268"/>
-      <c r="F10" s="268"/>
-      <c r="G10" s="268"/>
-      <c r="H10" s="268"/>
-      <c r="I10" s="268"/>
-      <c r="J10" s="268"/>
+      <c r="B10" s="254"/>
+      <c r="C10" s="254"/>
+      <c r="D10" s="254"/>
+      <c r="E10" s="254"/>
+      <c r="F10" s="254"/>
+      <c r="G10" s="254"/>
+      <c r="H10" s="254"/>
+      <c r="I10" s="254"/>
+      <c r="J10" s="254"/>
     </row>
     <row r="11" spans="1:99" ht="30.75" customHeight="1">
       <c r="F11" s="20" t="s">
@@ -13306,12 +13306,12 @@
       <c r="F21" s="24"/>
     </row>
     <row r="23" spans="6:7" ht="114.75" customHeight="1">
-      <c r="F23" s="269"/>
-      <c r="G23" s="269"/>
+      <c r="F23" s="255"/>
+      <c r="G23" s="255"/>
     </row>
     <row r="24" spans="6:7" ht="409.5" customHeight="1">
-      <c r="F24" s="264"/>
-      <c r="G24" s="264"/>
+      <c r="F24" s="245"/>
+      <c r="G24" s="245"/>
     </row>
     <row r="25" spans="6:7">
       <c r="F25" s="25"/>
@@ -13319,6 +13319,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="F7:J7"/>
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="F8:J8"/>
@@ -13326,19 +13339,6 @@
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="F23:G23"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F3:J3"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Organization You Represent" prompt="Please put the name of the HL7 member organization you represent if it is different from the name of the organization you are employed by.  " sqref="F6"/>
@@ -13365,10 +13365,10 @@
   <dimension ref="A1:AF713"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E166" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E197" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A166" sqref="A166"/>
+      <selection pane="bottomRight" activeCell="G526" sqref="G526"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -13408,43 +13408,43 @@
   <sheetData>
     <row r="1" spans="1:32" ht="17.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A1" s="32"/>
-      <c r="B1" s="270" t="s">
+      <c r="B1" s="271" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="271"/>
-      <c r="D1" s="271"/>
-      <c r="E1" s="271"/>
-      <c r="F1" s="271"/>
-      <c r="G1" s="271"/>
-      <c r="H1" s="272"/>
-      <c r="I1" s="273"/>
-      <c r="J1" s="273"/>
-      <c r="K1" s="274"/>
-      <c r="L1" s="272" t="s">
+      <c r="C1" s="272"/>
+      <c r="D1" s="272"/>
+      <c r="E1" s="272"/>
+      <c r="F1" s="272"/>
+      <c r="G1" s="272"/>
+      <c r="H1" s="273"/>
+      <c r="I1" s="274"/>
+      <c r="J1" s="274"/>
+      <c r="K1" s="275"/>
+      <c r="L1" s="273" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="273"/>
-      <c r="N1" s="273"/>
-      <c r="O1" s="273"/>
-      <c r="P1" s="273"/>
-      <c r="Q1" s="273"/>
-      <c r="R1" s="273"/>
-      <c r="S1" s="273"/>
-      <c r="T1" s="273"/>
-      <c r="U1" s="273"/>
-      <c r="V1" s="273"/>
-      <c r="W1" s="273"/>
-      <c r="X1" s="274"/>
-      <c r="Y1" s="272" t="s">
+      <c r="M1" s="274"/>
+      <c r="N1" s="274"/>
+      <c r="O1" s="274"/>
+      <c r="P1" s="274"/>
+      <c r="Q1" s="274"/>
+      <c r="R1" s="274"/>
+      <c r="S1" s="274"/>
+      <c r="T1" s="274"/>
+      <c r="U1" s="274"/>
+      <c r="V1" s="274"/>
+      <c r="W1" s="274"/>
+      <c r="X1" s="275"/>
+      <c r="Y1" s="273" t="s">
         <v>16</v>
       </c>
-      <c r="Z1" s="273"/>
-      <c r="AA1" s="273"/>
-      <c r="AB1" s="273"/>
-      <c r="AC1" s="273"/>
-      <c r="AD1" s="273"/>
-      <c r="AE1" s="273"/>
-      <c r="AF1" s="274"/>
+      <c r="Z1" s="274"/>
+      <c r="AA1" s="274"/>
+      <c r="AB1" s="274"/>
+      <c r="AC1" s="274"/>
+      <c r="AD1" s="274"/>
+      <c r="AE1" s="274"/>
+      <c r="AF1" s="275"/>
     </row>
     <row r="2" spans="1:32" s="33" customFormat="1" ht="41.25" customHeight="1" thickTop="1">
       <c r="A2" s="34" t="s">
@@ -27851,7 +27851,7 @@
       </c>
       <c r="E188" s="47"/>
       <c r="F188" s="47"/>
-      <c r="G188" s="338" t="s">
+      <c r="G188" s="244" t="s">
         <v>768</v>
       </c>
       <c r="H188" s="49"/>
@@ -27977,7 +27977,7 @@
       </c>
       <c r="E190" s="47"/>
       <c r="F190" s="47"/>
-      <c r="G190" s="338" t="s">
+      <c r="G190" s="244" t="s">
         <v>770</v>
       </c>
       <c r="H190" s="49"/>
@@ -29708,7 +29708,7 @@
       <c r="AE213" s="214"/>
       <c r="AF213" s="215"/>
     </row>
-    <row r="214" spans="1:32" s="60" customFormat="1" ht="25.5" customHeight="1">
+    <row r="214" spans="1:32" s="60" customFormat="1" ht="25.5" hidden="1" customHeight="1">
       <c r="A214" s="45">
         <v>212</v>
       </c>
@@ -29746,7 +29746,9 @@
       <c r="Q214" s="52" t="s">
         <v>820</v>
       </c>
-      <c r="R214" s="52"/>
+      <c r="R214" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S214" s="52"/>
       <c r="T214" s="53"/>
       <c r="U214" s="53"/>
@@ -29846,7 +29848,7 @@
       <c r="AE215" s="58"/>
       <c r="AF215" s="59"/>
     </row>
-    <row r="216" spans="1:32" s="60" customFormat="1" ht="25.5" customHeight="1">
+    <row r="216" spans="1:32" s="60" customFormat="1" ht="25.5" hidden="1" customHeight="1">
       <c r="A216" s="45">
         <v>214</v>
       </c>
@@ -29887,7 +29889,7 @@
         <v>82</v>
       </c>
       <c r="R216" s="52" t="s">
-        <v>2526</v>
+        <v>72</v>
       </c>
       <c r="S216" s="52"/>
       <c r="T216" s="53"/>
@@ -30260,7 +30262,7 @@
       <c r="AE221" s="58"/>
       <c r="AF221" s="59"/>
     </row>
-    <row r="222" spans="1:32" s="60" customFormat="1" ht="25.5" customHeight="1">
+    <row r="222" spans="1:32" s="60" customFormat="1" ht="25.5" hidden="1" customHeight="1">
       <c r="A222" s="45">
         <v>220</v>
       </c>
@@ -30300,7 +30302,9 @@
       <c r="Q222" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="R222" s="52"/>
+      <c r="R222" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S222" s="52"/>
       <c r="T222" s="53"/>
       <c r="U222" s="53"/>
@@ -30328,7 +30332,7 @@
       <c r="AE222" s="58"/>
       <c r="AF222" s="59"/>
     </row>
-    <row r="223" spans="1:32" s="60" customFormat="1" ht="25.5" customHeight="1">
+    <row r="223" spans="1:32" s="60" customFormat="1" ht="25.5" hidden="1" customHeight="1">
       <c r="A223" s="45">
         <v>221</v>
       </c>
@@ -30368,7 +30372,9 @@
       <c r="Q223" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="R223" s="52"/>
+      <c r="R223" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S223" s="52"/>
       <c r="T223" s="53"/>
       <c r="U223" s="53"/>
@@ -30432,7 +30438,9 @@
       <c r="Q224" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="R224" s="52"/>
+      <c r="R224" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S224" s="52"/>
       <c r="T224" s="53"/>
       <c r="U224" s="53"/>
@@ -30460,7 +30468,7 @@
       <c r="AE224" s="58"/>
       <c r="AF224" s="59"/>
     </row>
-    <row r="225" spans="1:32" s="60" customFormat="1" ht="38.25" customHeight="1">
+    <row r="225" spans="1:32" s="60" customFormat="1" ht="38.25" hidden="1" customHeight="1">
       <c r="A225" s="45">
         <v>223</v>
       </c>
@@ -30494,7 +30502,9 @@
       <c r="O225" s="50"/>
       <c r="P225" s="52"/>
       <c r="Q225" s="52"/>
-      <c r="R225" s="52"/>
+      <c r="R225" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S225" s="52"/>
       <c r="T225" s="53"/>
       <c r="U225" s="53"/>
@@ -30590,7 +30600,7 @@
       <c r="AE226" s="58"/>
       <c r="AF226" s="59"/>
     </row>
-    <row r="227" spans="1:32" s="60" customFormat="1" ht="51" customHeight="1">
+    <row r="227" spans="1:32" s="60" customFormat="1" ht="51" hidden="1" customHeight="1">
       <c r="A227" s="45">
         <v>225</v>
       </c>
@@ -30626,7 +30636,9 @@
       <c r="O227" s="50"/>
       <c r="P227" s="52"/>
       <c r="Q227" s="52"/>
-      <c r="R227" s="52"/>
+      <c r="R227" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S227" s="52"/>
       <c r="T227" s="53"/>
       <c r="U227" s="53"/>
@@ -30718,7 +30730,7 @@
       <c r="AE228" s="58"/>
       <c r="AF228" s="59"/>
     </row>
-    <row r="229" spans="1:32" s="60" customFormat="1" ht="25.5" customHeight="1">
+    <row r="229" spans="1:32" s="60" customFormat="1" ht="25.5" hidden="1" customHeight="1">
       <c r="A229" s="45">
         <v>227</v>
       </c>
@@ -30754,7 +30766,9 @@
       <c r="O229" s="50"/>
       <c r="P229" s="52"/>
       <c r="Q229" s="52"/>
-      <c r="R229" s="52"/>
+      <c r="R229" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S229" s="52"/>
       <c r="T229" s="53"/>
       <c r="U229" s="53"/>
@@ -30782,7 +30796,7 @@
       <c r="AE229" s="58"/>
       <c r="AF229" s="59"/>
     </row>
-    <row r="230" spans="1:32" s="60" customFormat="1" ht="63.75" customHeight="1">
+    <row r="230" spans="1:32" s="60" customFormat="1" ht="63.75" hidden="1" customHeight="1">
       <c r="A230" s="64">
         <v>228</v>
       </c>
@@ -30822,7 +30836,9 @@
       <c r="Q230" s="52" t="s">
         <v>857</v>
       </c>
-      <c r="R230" s="52"/>
+      <c r="R230" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S230" s="52"/>
       <c r="T230" s="53"/>
       <c r="U230" s="53"/>
@@ -49868,7 +49884,7 @@
       <c r="AE501" s="58"/>
       <c r="AF501" s="68"/>
     </row>
-    <row r="502" spans="1:32" ht="38.25" customHeight="1">
+    <row r="502" spans="1:32" ht="38.25" hidden="1" customHeight="1">
       <c r="A502" s="64">
         <v>499</v>
       </c>
@@ -49906,7 +49922,9 @@
       <c r="Q502" s="52" t="s">
         <v>82</v>
       </c>
-      <c r="R502" s="52"/>
+      <c r="R502" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S502" s="52"/>
       <c r="T502" s="53"/>
       <c r="U502" s="53"/>
@@ -60314,7 +60332,7 @@
       <c r="AE645" s="58"/>
       <c r="AF645" s="68"/>
     </row>
-    <row r="646" spans="1:32" ht="25.5" customHeight="1">
+    <row r="646" spans="1:32" ht="25.5" hidden="1" customHeight="1">
       <c r="A646" s="64">
         <v>643</v>
       </c>
@@ -60352,7 +60370,9 @@
       <c r="Q646" s="52" t="s">
         <v>2030</v>
       </c>
-      <c r="R646" s="52"/>
+      <c r="R646" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S646" s="52"/>
       <c r="T646" s="53"/>
       <c r="U646" s="53"/>
@@ -65840,10 +65860,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="13.5" customHeight="1" thickBot="1">
-      <c r="H1" s="277" t="s">
+      <c r="H1" s="317" t="s">
         <v>2237</v>
       </c>
-      <c r="I1" s="277"/>
+      <c r="I1" s="317"/>
     </row>
     <row r="2" spans="2:14" ht="15.75" customHeight="1">
       <c r="B2" s="75" t="s">
@@ -65858,16 +65878,16 @@
       <c r="I2" s="77"/>
     </row>
     <row r="3" spans="2:14" ht="303.75" customHeight="1" thickBot="1">
-      <c r="B3" s="278" t="s">
+      <c r="B3" s="318" t="s">
         <v>2239</v>
       </c>
-      <c r="C3" s="279"/>
-      <c r="D3" s="279"/>
-      <c r="E3" s="279"/>
-      <c r="F3" s="279"/>
-      <c r="G3" s="279"/>
-      <c r="H3" s="279"/>
-      <c r="I3" s="280"/>
+      <c r="C3" s="319"/>
+      <c r="D3" s="319"/>
+      <c r="E3" s="319"/>
+      <c r="F3" s="319"/>
+      <c r="G3" s="319"/>
+      <c r="H3" s="319"/>
+      <c r="I3" s="320"/>
     </row>
     <row r="4" spans="2:14" ht="13.5" customHeight="1" thickBot="1">
       <c r="J4" s="25"/>
@@ -65885,16 +65905,16 @@
       <c r="I5" s="77"/>
     </row>
     <row r="6" spans="2:14" ht="18" customHeight="1">
-      <c r="B6" s="281" t="s">
+      <c r="B6" s="300" t="s">
         <v>2241</v>
       </c>
-      <c r="C6" s="282"/>
-      <c r="D6" s="282"/>
-      <c r="E6" s="282"/>
-      <c r="F6" s="282"/>
-      <c r="G6" s="282"/>
-      <c r="H6" s="282"/>
-      <c r="I6" s="283"/>
+      <c r="C6" s="301"/>
+      <c r="D6" s="301"/>
+      <c r="E6" s="301"/>
+      <c r="F6" s="301"/>
+      <c r="G6" s="301"/>
+      <c r="H6" s="301"/>
+      <c r="I6" s="302"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -65904,15 +65924,15 @@
       <c r="B7" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="284" t="s">
+      <c r="C7" s="321" t="s">
         <v>2242</v>
       </c>
-      <c r="D7" s="285"/>
-      <c r="E7" s="285"/>
-      <c r="F7" s="285"/>
-      <c r="G7" s="285"/>
-      <c r="H7" s="285"/>
-      <c r="I7" s="286"/>
+      <c r="D7" s="322"/>
+      <c r="E7" s="322"/>
+      <c r="F7" s="322"/>
+      <c r="G7" s="322"/>
+      <c r="H7" s="322"/>
+      <c r="I7" s="323"/>
       <c r="J7" s="79"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -65922,15 +65942,15 @@
       <c r="B8" s="80" t="s">
         <v>2243</v>
       </c>
-      <c r="C8" s="287" t="s">
+      <c r="C8" s="324" t="s">
         <v>2244</v>
       </c>
-      <c r="D8" s="287"/>
-      <c r="E8" s="287"/>
-      <c r="F8" s="287"/>
-      <c r="G8" s="287"/>
-      <c r="H8" s="287"/>
-      <c r="I8" s="288"/>
+      <c r="D8" s="324"/>
+      <c r="E8" s="324"/>
+      <c r="F8" s="324"/>
+      <c r="G8" s="324"/>
+      <c r="H8" s="324"/>
+      <c r="I8" s="325"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -65940,15 +65960,15 @@
       <c r="B9" s="81" t="s">
         <v>2245</v>
       </c>
-      <c r="C9" s="275" t="s">
+      <c r="C9" s="315" t="s">
         <v>2246</v>
       </c>
-      <c r="D9" s="275"/>
-      <c r="E9" s="275"/>
-      <c r="F9" s="275"/>
-      <c r="G9" s="275"/>
-      <c r="H9" s="275"/>
-      <c r="I9" s="276"/>
+      <c r="D9" s="315"/>
+      <c r="E9" s="315"/>
+      <c r="F9" s="315"/>
+      <c r="G9" s="315"/>
+      <c r="H9" s="315"/>
+      <c r="I9" s="316"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -65959,13 +65979,13 @@
       <c r="C10" s="83" t="s">
         <v>2247</v>
       </c>
-      <c r="D10" s="290" t="s">
+      <c r="D10" s="313" t="s">
         <v>2248</v>
       </c>
-      <c r="E10" s="291"/>
-      <c r="F10" s="291"/>
-      <c r="G10" s="291"/>
-      <c r="H10" s="292"/>
+      <c r="E10" s="292"/>
+      <c r="F10" s="292"/>
+      <c r="G10" s="292"/>
+      <c r="H10" s="314"/>
       <c r="I10" s="84"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -65977,13 +65997,13 @@
       <c r="C11" s="83" t="s">
         <v>2249</v>
       </c>
-      <c r="D11" s="290" t="s">
+      <c r="D11" s="313" t="s">
         <v>2250</v>
       </c>
-      <c r="E11" s="291"/>
-      <c r="F11" s="291"/>
-      <c r="G11" s="291"/>
-      <c r="H11" s="292"/>
+      <c r="E11" s="292"/>
+      <c r="F11" s="292"/>
+      <c r="G11" s="292"/>
+      <c r="H11" s="314"/>
       <c r="I11" s="84"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -65996,13 +66016,13 @@
       <c r="C12" s="83" t="s">
         <v>2251</v>
       </c>
-      <c r="D12" s="290" t="s">
+      <c r="D12" s="313" t="s">
         <v>2252</v>
       </c>
-      <c r="E12" s="291"/>
-      <c r="F12" s="291"/>
-      <c r="G12" s="291"/>
-      <c r="H12" s="292"/>
+      <c r="E12" s="292"/>
+      <c r="F12" s="292"/>
+      <c r="G12" s="292"/>
+      <c r="H12" s="314"/>
       <c r="I12" s="84"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -66014,13 +66034,13 @@
       <c r="C13" s="83" t="s">
         <v>2253</v>
       </c>
-      <c r="D13" s="290" t="s">
+      <c r="D13" s="313" t="s">
         <v>2254</v>
       </c>
-      <c r="E13" s="291"/>
-      <c r="F13" s="291"/>
-      <c r="G13" s="291"/>
-      <c r="H13" s="292"/>
+      <c r="E13" s="292"/>
+      <c r="F13" s="292"/>
+      <c r="G13" s="292"/>
+      <c r="H13" s="314"/>
       <c r="I13" s="84"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -66032,13 +66052,13 @@
       <c r="C14" s="83" t="s">
         <v>2255</v>
       </c>
-      <c r="D14" s="290" t="s">
+      <c r="D14" s="313" t="s">
         <v>2256</v>
       </c>
-      <c r="E14" s="291"/>
-      <c r="F14" s="291"/>
-      <c r="G14" s="291"/>
-      <c r="H14" s="292"/>
+      <c r="E14" s="292"/>
+      <c r="F14" s="292"/>
+      <c r="G14" s="292"/>
+      <c r="H14" s="314"/>
       <c r="I14" s="84"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -66050,13 +66070,13 @@
       <c r="C15" s="83" t="s">
         <v>2257</v>
       </c>
-      <c r="D15" s="290" t="s">
+      <c r="D15" s="313" t="s">
         <v>2258</v>
       </c>
-      <c r="E15" s="291"/>
-      <c r="F15" s="291"/>
-      <c r="G15" s="291"/>
-      <c r="H15" s="292"/>
+      <c r="E15" s="292"/>
+      <c r="F15" s="292"/>
+      <c r="G15" s="292"/>
+      <c r="H15" s="314"/>
       <c r="I15" s="84"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -66068,13 +66088,13 @@
       <c r="C16" s="83" t="s">
         <v>2259</v>
       </c>
-      <c r="D16" s="290" t="s">
+      <c r="D16" s="313" t="s">
         <v>2260</v>
       </c>
-      <c r="E16" s="291"/>
-      <c r="F16" s="291"/>
-      <c r="G16" s="291"/>
-      <c r="H16" s="292"/>
+      <c r="E16" s="292"/>
+      <c r="F16" s="292"/>
+      <c r="G16" s="292"/>
+      <c r="H16" s="314"/>
       <c r="I16" s="84"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -66086,13 +66106,13 @@
       <c r="C17" s="83" t="s">
         <v>2261</v>
       </c>
-      <c r="D17" s="290" t="s">
+      <c r="D17" s="313" t="s">
         <v>2262</v>
       </c>
-      <c r="E17" s="291"/>
-      <c r="F17" s="291"/>
-      <c r="G17" s="291"/>
-      <c r="H17" s="292"/>
+      <c r="E17" s="292"/>
+      <c r="F17" s="292"/>
+      <c r="G17" s="292"/>
+      <c r="H17" s="314"/>
       <c r="I17" s="84"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -66104,13 +66124,13 @@
       <c r="C18" s="83" t="s">
         <v>2263</v>
       </c>
-      <c r="D18" s="290" t="s">
+      <c r="D18" s="313" t="s">
         <v>2264</v>
       </c>
-      <c r="E18" s="291"/>
-      <c r="F18" s="291"/>
-      <c r="G18" s="291"/>
-      <c r="H18" s="292"/>
+      <c r="E18" s="292"/>
+      <c r="F18" s="292"/>
+      <c r="G18" s="292"/>
+      <c r="H18" s="314"/>
       <c r="I18" s="84"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -66135,15 +66155,15 @@
       <c r="B20" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="293" t="s">
+      <c r="C20" s="296" t="s">
         <v>2265</v>
       </c>
-      <c r="D20" s="293"/>
-      <c r="E20" s="293"/>
-      <c r="F20" s="293"/>
-      <c r="G20" s="293"/>
-      <c r="H20" s="293"/>
-      <c r="I20" s="294"/>
+      <c r="D20" s="296"/>
+      <c r="E20" s="296"/>
+      <c r="F20" s="296"/>
+      <c r="G20" s="296"/>
+      <c r="H20" s="296"/>
+      <c r="I20" s="297"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -66153,33 +66173,33 @@
       <c r="B21" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="291" t="s">
+      <c r="C21" s="292" t="s">
         <v>2266</v>
       </c>
-      <c r="D21" s="291"/>
-      <c r="E21" s="291"/>
-      <c r="F21" s="291"/>
-      <c r="G21" s="291"/>
-      <c r="H21" s="291"/>
-      <c r="I21" s="295"/>
+      <c r="D21" s="292"/>
+      <c r="E21" s="292"/>
+      <c r="F21" s="292"/>
+      <c r="G21" s="292"/>
+      <c r="H21" s="292"/>
+      <c r="I21" s="293"/>
       <c r="J21" s="89"/>
-      <c r="K21" s="289"/>
-      <c r="L21" s="289"/>
-      <c r="M21" s="289"/>
+      <c r="K21" s="312"/>
+      <c r="L21" s="312"/>
+      <c r="M21" s="312"/>
     </row>
     <row r="22" spans="2:13" ht="27.75" customHeight="1">
       <c r="B22" s="80" t="s">
         <v>2267</v>
       </c>
-      <c r="C22" s="291" t="s">
+      <c r="C22" s="292" t="s">
         <v>2268</v>
       </c>
-      <c r="D22" s="291"/>
-      <c r="E22" s="291"/>
-      <c r="F22" s="291"/>
-      <c r="G22" s="291"/>
-      <c r="H22" s="291"/>
-      <c r="I22" s="295"/>
+      <c r="D22" s="292"/>
+      <c r="E22" s="292"/>
+      <c r="F22" s="292"/>
+      <c r="G22" s="292"/>
+      <c r="H22" s="292"/>
+      <c r="I22" s="293"/>
       <c r="J22" s="89"/>
       <c r="K22" s="90"/>
       <c r="L22" s="90"/>
@@ -66189,45 +66209,45 @@
       <c r="B23" s="80" t="s">
         <v>2269</v>
       </c>
-      <c r="C23" s="298" t="s">
+      <c r="C23" s="294" t="s">
         <v>2270</v>
       </c>
-      <c r="D23" s="298"/>
-      <c r="E23" s="298"/>
-      <c r="F23" s="298"/>
-      <c r="G23" s="298"/>
-      <c r="H23" s="298"/>
-      <c r="I23" s="299"/>
+      <c r="D23" s="294"/>
+      <c r="E23" s="294"/>
+      <c r="F23" s="294"/>
+      <c r="G23" s="294"/>
+      <c r="H23" s="294"/>
+      <c r="I23" s="295"/>
       <c r="M23" s="2"/>
     </row>
     <row r="24" spans="2:13" ht="18" customHeight="1">
       <c r="B24" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="293" t="s">
+      <c r="C24" s="296" t="s">
         <v>2271</v>
       </c>
-      <c r="D24" s="293"/>
-      <c r="E24" s="293"/>
-      <c r="F24" s="293"/>
-      <c r="G24" s="293"/>
-      <c r="H24" s="293"/>
-      <c r="I24" s="294"/>
+      <c r="D24" s="296"/>
+      <c r="E24" s="296"/>
+      <c r="F24" s="296"/>
+      <c r="G24" s="296"/>
+      <c r="H24" s="296"/>
+      <c r="I24" s="297"/>
       <c r="M24" s="2"/>
     </row>
     <row r="25" spans="2:13" ht="15.75" customHeight="1">
       <c r="B25" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="293" t="s">
+      <c r="C25" s="296" t="s">
         <v>2272</v>
       </c>
-      <c r="D25" s="293"/>
-      <c r="E25" s="293"/>
-      <c r="F25" s="293"/>
-      <c r="G25" s="293"/>
-      <c r="H25" s="293"/>
-      <c r="I25" s="294"/>
+      <c r="D25" s="296"/>
+      <c r="E25" s="296"/>
+      <c r="F25" s="296"/>
+      <c r="G25" s="296"/>
+      <c r="H25" s="296"/>
+      <c r="I25" s="297"/>
       <c r="J25" s="91"/>
       <c r="M25" s="2"/>
     </row>
@@ -66235,15 +66255,15 @@
       <c r="B26" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="293" t="s">
+      <c r="C26" s="296" t="s">
         <v>2273</v>
       </c>
-      <c r="D26" s="293"/>
-      <c r="E26" s="293"/>
-      <c r="F26" s="293"/>
-      <c r="G26" s="293"/>
-      <c r="H26" s="293"/>
-      <c r="I26" s="294"/>
+      <c r="D26" s="296"/>
+      <c r="E26" s="296"/>
+      <c r="F26" s="296"/>
+      <c r="G26" s="296"/>
+      <c r="H26" s="296"/>
+      <c r="I26" s="297"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -66253,28 +66273,28 @@
       <c r="B27" s="92" t="s">
         <v>2274</v>
       </c>
-      <c r="C27" s="300" t="s">
+      <c r="C27" s="298" t="s">
         <v>2275</v>
       </c>
-      <c r="D27" s="300"/>
-      <c r="E27" s="300"/>
-      <c r="F27" s="300"/>
-      <c r="G27" s="300"/>
-      <c r="H27" s="300"/>
-      <c r="I27" s="301"/>
+      <c r="D27" s="298"/>
+      <c r="E27" s="298"/>
+      <c r="F27" s="298"/>
+      <c r="G27" s="298"/>
+      <c r="H27" s="298"/>
+      <c r="I27" s="299"/>
       <c r="J27" s="25"/>
     </row>
     <row r="28" spans="2:13" ht="18" customHeight="1">
-      <c r="B28" s="281" t="s">
+      <c r="B28" s="300" t="s">
         <v>2276</v>
       </c>
-      <c r="C28" s="282"/>
-      <c r="D28" s="282"/>
-      <c r="E28" s="282"/>
-      <c r="F28" s="282"/>
-      <c r="G28" s="282"/>
-      <c r="H28" s="282"/>
-      <c r="I28" s="283"/>
+      <c r="C28" s="301"/>
+      <c r="D28" s="301"/>
+      <c r="E28" s="301"/>
+      <c r="F28" s="301"/>
+      <c r="G28" s="301"/>
+      <c r="H28" s="301"/>
+      <c r="I28" s="302"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -66284,15 +66304,15 @@
       <c r="B29" s="93" t="s">
         <v>2277</v>
       </c>
-      <c r="C29" s="302" t="s">
+      <c r="C29" s="303" t="s">
         <v>2278</v>
       </c>
-      <c r="D29" s="303"/>
-      <c r="E29" s="303"/>
-      <c r="F29" s="303"/>
-      <c r="G29" s="303"/>
-      <c r="H29" s="303"/>
-      <c r="I29" s="304"/>
+      <c r="D29" s="304"/>
+      <c r="E29" s="304"/>
+      <c r="F29" s="304"/>
+      <c r="G29" s="304"/>
+      <c r="H29" s="304"/>
+      <c r="I29" s="305"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
@@ -66302,15 +66322,15 @@
       <c r="B30" s="94" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="305" t="s">
+      <c r="C30" s="306" t="s">
         <v>2279</v>
       </c>
-      <c r="D30" s="306"/>
-      <c r="E30" s="306"/>
-      <c r="F30" s="306"/>
-      <c r="G30" s="306"/>
-      <c r="H30" s="306"/>
-      <c r="I30" s="307"/>
+      <c r="D30" s="307"/>
+      <c r="E30" s="307"/>
+      <c r="F30" s="307"/>
+      <c r="G30" s="307"/>
+      <c r="H30" s="307"/>
+      <c r="I30" s="308"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -66320,15 +66340,15 @@
       <c r="B31" s="93" t="s">
         <v>2280</v>
       </c>
-      <c r="C31" s="308" t="s">
+      <c r="C31" s="309" t="s">
         <v>2281</v>
       </c>
-      <c r="D31" s="309"/>
-      <c r="E31" s="309"/>
-      <c r="F31" s="309"/>
-      <c r="G31" s="309"/>
-      <c r="H31" s="309"/>
-      <c r="I31" s="310"/>
+      <c r="D31" s="310"/>
+      <c r="E31" s="310"/>
+      <c r="F31" s="310"/>
+      <c r="G31" s="310"/>
+      <c r="H31" s="310"/>
+      <c r="I31" s="311"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
@@ -66338,15 +66358,15 @@
       <c r="B32" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="296" t="s">
+      <c r="C32" s="290" t="s">
         <v>2282</v>
       </c>
-      <c r="D32" s="296"/>
-      <c r="E32" s="296"/>
-      <c r="F32" s="296"/>
-      <c r="G32" s="296"/>
-      <c r="H32" s="296"/>
-      <c r="I32" s="297"/>
+      <c r="D32" s="290"/>
+      <c r="E32" s="290"/>
+      <c r="F32" s="290"/>
+      <c r="G32" s="290"/>
+      <c r="H32" s="290"/>
+      <c r="I32" s="291"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -66356,15 +66376,15 @@
       <c r="B33" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="296" t="s">
+      <c r="C33" s="290" t="s">
         <v>2283</v>
       </c>
-      <c r="D33" s="296"/>
-      <c r="E33" s="296"/>
-      <c r="F33" s="296"/>
-      <c r="G33" s="296"/>
-      <c r="H33" s="296"/>
-      <c r="I33" s="297"/>
+      <c r="D33" s="290"/>
+      <c r="E33" s="290"/>
+      <c r="F33" s="290"/>
+      <c r="G33" s="290"/>
+      <c r="H33" s="290"/>
+      <c r="I33" s="291"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -66374,15 +66394,15 @@
       <c r="B34" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="314" t="s">
+      <c r="C34" s="279" t="s">
         <v>2284</v>
       </c>
-      <c r="D34" s="314"/>
-      <c r="E34" s="314"/>
-      <c r="F34" s="314"/>
-      <c r="G34" s="314"/>
-      <c r="H34" s="314"/>
-      <c r="I34" s="315"/>
+      <c r="D34" s="279"/>
+      <c r="E34" s="279"/>
+      <c r="F34" s="279"/>
+      <c r="G34" s="279"/>
+      <c r="H34" s="279"/>
+      <c r="I34" s="280"/>
       <c r="J34" s="2"/>
       <c r="K34" s="90"/>
       <c r="L34" s="90"/>
@@ -66392,15 +66412,15 @@
       <c r="B35" s="96" t="s">
         <v>2285</v>
       </c>
-      <c r="C35" s="314" t="s">
+      <c r="C35" s="279" t="s">
         <v>2286</v>
       </c>
-      <c r="D35" s="314"/>
-      <c r="E35" s="314"/>
-      <c r="F35" s="314"/>
-      <c r="G35" s="314"/>
-      <c r="H35" s="314"/>
-      <c r="I35" s="315"/>
+      <c r="D35" s="279"/>
+      <c r="E35" s="279"/>
+      <c r="F35" s="279"/>
+      <c r="G35" s="279"/>
+      <c r="H35" s="279"/>
+      <c r="I35" s="280"/>
       <c r="J35" s="2"/>
       <c r="K35" s="90"/>
       <c r="L35" s="90"/>
@@ -66410,15 +66430,15 @@
       <c r="B36" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="314" t="s">
+      <c r="C36" s="279" t="s">
         <v>2287</v>
       </c>
-      <c r="D36" s="314"/>
-      <c r="E36" s="314"/>
-      <c r="F36" s="314"/>
-      <c r="G36" s="314"/>
-      <c r="H36" s="314"/>
-      <c r="I36" s="315"/>
+      <c r="D36" s="279"/>
+      <c r="E36" s="279"/>
+      <c r="F36" s="279"/>
+      <c r="G36" s="279"/>
+      <c r="H36" s="279"/>
+      <c r="I36" s="280"/>
       <c r="J36" s="2"/>
       <c r="K36" s="90"/>
       <c r="L36" s="90"/>
@@ -66428,15 +66448,15 @@
       <c r="B37" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="314" t="s">
+      <c r="C37" s="279" t="s">
         <v>2288</v>
       </c>
-      <c r="D37" s="314"/>
-      <c r="E37" s="314"/>
-      <c r="F37" s="314"/>
-      <c r="G37" s="314"/>
-      <c r="H37" s="314"/>
-      <c r="I37" s="315"/>
+      <c r="D37" s="279"/>
+      <c r="E37" s="279"/>
+      <c r="F37" s="279"/>
+      <c r="G37" s="279"/>
+      <c r="H37" s="279"/>
+      <c r="I37" s="280"/>
       <c r="J37" s="2"/>
       <c r="K37" s="90"/>
       <c r="L37" s="90"/>
@@ -66446,116 +66466,146 @@
       <c r="B38" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="316" t="s">
+      <c r="C38" s="281" t="s">
         <v>2289</v>
       </c>
-      <c r="D38" s="317"/>
-      <c r="E38" s="317"/>
-      <c r="F38" s="317"/>
-      <c r="G38" s="317"/>
-      <c r="H38" s="317"/>
-      <c r="I38" s="318"/>
+      <c r="D38" s="282"/>
+      <c r="E38" s="282"/>
+      <c r="F38" s="282"/>
+      <c r="G38" s="282"/>
+      <c r="H38" s="282"/>
+      <c r="I38" s="283"/>
     </row>
     <row r="39" spans="2:13" ht="54.75" customHeight="1" thickBot="1">
       <c r="B39" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="316" t="s">
+      <c r="C39" s="281" t="s">
         <v>2290</v>
       </c>
-      <c r="D39" s="317"/>
-      <c r="E39" s="317"/>
-      <c r="F39" s="317"/>
-      <c r="G39" s="317"/>
-      <c r="H39" s="317"/>
-      <c r="I39" s="318"/>
+      <c r="D39" s="282"/>
+      <c r="E39" s="282"/>
+      <c r="F39" s="282"/>
+      <c r="G39" s="282"/>
+      <c r="H39" s="282"/>
+      <c r="I39" s="283"/>
     </row>
     <row r="40" spans="2:13" ht="40.5" customHeight="1" thickBot="1">
       <c r="B40" s="100" t="s">
         <v>2291</v>
       </c>
-      <c r="C40" s="319" t="s">
+      <c r="C40" s="284" t="s">
         <v>2292</v>
       </c>
-      <c r="D40" s="320"/>
-      <c r="E40" s="320"/>
-      <c r="F40" s="320"/>
-      <c r="G40" s="320"/>
-      <c r="H40" s="320"/>
-      <c r="I40" s="321"/>
+      <c r="D40" s="285"/>
+      <c r="E40" s="285"/>
+      <c r="F40" s="285"/>
+      <c r="G40" s="285"/>
+      <c r="H40" s="285"/>
+      <c r="I40" s="286"/>
     </row>
     <row r="41" spans="2:13" ht="40.5" customHeight="1" thickBot="1">
       <c r="B41" s="101" t="s">
         <v>2293</v>
       </c>
-      <c r="C41" s="322" t="s">
+      <c r="C41" s="287" t="s">
         <v>2294</v>
       </c>
-      <c r="D41" s="320"/>
-      <c r="E41" s="320"/>
-      <c r="F41" s="320"/>
-      <c r="G41" s="320"/>
-      <c r="H41" s="320"/>
-      <c r="I41" s="321"/>
+      <c r="D41" s="285"/>
+      <c r="E41" s="285"/>
+      <c r="F41" s="285"/>
+      <c r="G41" s="285"/>
+      <c r="H41" s="285"/>
+      <c r="I41" s="286"/>
     </row>
     <row r="42" spans="2:13" ht="40.5" customHeight="1" thickBot="1">
       <c r="B42" s="102" t="s">
         <v>2295</v>
       </c>
-      <c r="C42" s="323" t="s">
+      <c r="C42" s="288" t="s">
         <v>2296</v>
       </c>
-      <c r="D42" s="323"/>
-      <c r="E42" s="323"/>
-      <c r="F42" s="323"/>
-      <c r="G42" s="323"/>
-      <c r="H42" s="323"/>
-      <c r="I42" s="324"/>
+      <c r="D42" s="288"/>
+      <c r="E42" s="288"/>
+      <c r="F42" s="288"/>
+      <c r="G42" s="288"/>
+      <c r="H42" s="288"/>
+      <c r="I42" s="289"/>
     </row>
     <row r="43" spans="2:13" ht="43.5" customHeight="1" thickBot="1">
       <c r="B43" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="311" t="s">
+      <c r="C43" s="276" t="s">
         <v>2297</v>
       </c>
-      <c r="D43" s="312"/>
-      <c r="E43" s="312"/>
-      <c r="F43" s="312"/>
-      <c r="G43" s="312"/>
-      <c r="H43" s="312"/>
-      <c r="I43" s="313"/>
+      <c r="D43" s="277"/>
+      <c r="E43" s="277"/>
+      <c r="F43" s="277"/>
+      <c r="G43" s="277"/>
+      <c r="H43" s="277"/>
+      <c r="I43" s="278"/>
     </row>
     <row r="44" spans="2:13" ht="13.5" customHeight="1" thickBot="1">
       <c r="B44" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="311" t="s">
+      <c r="C44" s="276" t="s">
         <v>2298</v>
       </c>
-      <c r="D44" s="312"/>
-      <c r="E44" s="312"/>
-      <c r="F44" s="312"/>
-      <c r="G44" s="312"/>
-      <c r="H44" s="312"/>
-      <c r="I44" s="313"/>
+      <c r="D44" s="277"/>
+      <c r="E44" s="277"/>
+      <c r="F44" s="277"/>
+      <c r="G44" s="277"/>
+      <c r="H44" s="277"/>
+      <c r="I44" s="278"/>
     </row>
     <row r="45" spans="2:13" ht="32.25" customHeight="1" thickBot="1">
       <c r="B45" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="311" t="s">
+      <c r="C45" s="276" t="s">
         <v>2299</v>
       </c>
-      <c r="D45" s="312"/>
-      <c r="E45" s="312"/>
-      <c r="F45" s="312"/>
-      <c r="G45" s="312"/>
-      <c r="H45" s="312"/>
-      <c r="I45" s="313"/>
+      <c r="D45" s="277"/>
+      <c r="E45" s="277"/>
+      <c r="F45" s="277"/>
+      <c r="G45" s="277"/>
+      <c r="H45" s="277"/>
+      <c r="I45" s="278"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
     <mergeCell ref="C45:I45"/>
     <mergeCell ref="C34:I34"/>
     <mergeCell ref="C35:I35"/>
@@ -66568,36 +66618,6 @@
     <mergeCell ref="C42:I42"/>
     <mergeCell ref="C43:I43"/>
     <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="D16:H16"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C8:I8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H1" location="Ballot!A1" display="Ballot!A1"/>
@@ -66635,17 +66655,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.5" customHeight="1" thickTop="1">
-      <c r="A1" s="325" t="s">
+      <c r="A1" s="326" t="s">
         <v>2300</v>
       </c>
-      <c r="B1" s="326"/>
-      <c r="C1" s="326"/>
-      <c r="D1" s="326"/>
-      <c r="E1" s="326"/>
-      <c r="F1" s="326"/>
-      <c r="G1" s="326"/>
-      <c r="H1" s="326"/>
-      <c r="I1" s="326"/>
+      <c r="B1" s="327"/>
+      <c r="C1" s="327"/>
+      <c r="D1" s="327"/>
+      <c r="E1" s="327"/>
+      <c r="F1" s="327"/>
+      <c r="G1" s="327"/>
+      <c r="H1" s="327"/>
+      <c r="I1" s="327"/>
       <c r="J1" s="104" t="s">
         <v>2301</v>
       </c>
@@ -66656,15 +66676,15 @@
       <c r="M1" s="106"/>
     </row>
     <row r="2" spans="1:13" ht="13.5" customHeight="1" thickBot="1">
-      <c r="A2" s="327"/>
-      <c r="B2" s="328"/>
-      <c r="C2" s="328"/>
-      <c r="D2" s="328"/>
-      <c r="E2" s="328"/>
-      <c r="F2" s="328"/>
-      <c r="G2" s="328"/>
-      <c r="H2" s="328"/>
-      <c r="I2" s="328"/>
+      <c r="A2" s="328"/>
+      <c r="B2" s="329"/>
+      <c r="C2" s="329"/>
+      <c r="D2" s="329"/>
+      <c r="E2" s="329"/>
+      <c r="F2" s="329"/>
+      <c r="G2" s="329"/>
+      <c r="H2" s="329"/>
+      <c r="I2" s="329"/>
       <c r="J2" s="107"/>
       <c r="K2" s="107"/>
       <c r="L2" s="107"/>
@@ -68334,7 +68354,7 @@
       <c r="D2" s="123"/>
     </row>
     <row r="3" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A3" s="329" t="s">
+      <c r="A3" s="330" t="s">
         <v>2308</v>
       </c>
       <c r="B3" s="332" t="s">
@@ -68351,7 +68371,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A4" s="330"/>
+      <c r="A4" s="331"/>
       <c r="B4" s="333"/>
       <c r="C4" s="124" t="s">
         <v>2313</v>
@@ -68364,7 +68384,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A5" s="330"/>
+      <c r="A5" s="331"/>
       <c r="B5" s="333"/>
       <c r="C5" s="124" t="s">
         <v>2316</v>
@@ -68377,7 +68397,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A6" s="330"/>
+      <c r="A6" s="331"/>
       <c r="B6" s="333"/>
       <c r="C6" s="124" t="s">
         <v>2318</v>
@@ -68390,7 +68410,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A7" s="330"/>
+      <c r="A7" s="331"/>
       <c r="B7" s="333"/>
       <c r="C7" s="124" t="s">
         <v>2257</v>
@@ -68403,7 +68423,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A8" s="330"/>
+      <c r="A8" s="331"/>
       <c r="B8" s="333"/>
       <c r="C8" s="124" t="s">
         <v>2321</v>
@@ -68416,7 +68436,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A9" s="330"/>
+      <c r="A9" s="331"/>
       <c r="B9" s="333"/>
       <c r="C9" s="124" t="s">
         <v>2324</v>
@@ -68429,7 +68449,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A10" s="330"/>
+      <c r="A10" s="331"/>
       <c r="B10" s="333"/>
       <c r="C10" s="124" t="s">
         <v>2326</v>
@@ -68442,7 +68462,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A11" s="331"/>
+      <c r="A11" s="338"/>
       <c r="B11" s="334"/>
       <c r="C11" s="124" t="s">
         <v>2329</v>
@@ -68524,10 +68544,10 @@
       <c r="D18" s="123"/>
     </row>
     <row r="19" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A19" s="329" t="s">
+      <c r="A19" s="330" t="s">
         <v>1150</v>
       </c>
-      <c r="B19" s="329" t="s">
+      <c r="B19" s="330" t="s">
         <v>2342</v>
       </c>
       <c r="C19" s="124" t="s">
@@ -68541,8 +68561,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A20" s="330"/>
-      <c r="B20" s="330"/>
+      <c r="A20" s="331"/>
+      <c r="B20" s="331"/>
       <c r="C20" s="124" t="s">
         <v>2345</v>
       </c>
@@ -68554,8 +68574,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A21" s="330"/>
-      <c r="B21" s="330"/>
+      <c r="A21" s="331"/>
+      <c r="B21" s="331"/>
       <c r="C21" s="124" t="s">
         <v>2347</v>
       </c>
@@ -68572,10 +68592,10 @@
       <c r="D22" s="123"/>
     </row>
     <row r="23" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A23" s="329" t="s">
+      <c r="A23" s="330" t="s">
         <v>2349</v>
       </c>
-      <c r="B23" s="329" t="s">
+      <c r="B23" s="330" t="s">
         <v>2350</v>
       </c>
       <c r="C23" s="124" t="s">
@@ -68589,8 +68609,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A24" s="330"/>
-      <c r="B24" s="330"/>
+      <c r="A24" s="331"/>
+      <c r="B24" s="331"/>
       <c r="C24" s="124" t="s">
         <v>2349</v>
       </c>
@@ -68607,7 +68627,7 @@
       <c r="D25" s="123"/>
     </row>
     <row r="26" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A26" s="329" t="s">
+      <c r="A26" s="330" t="s">
         <v>2354</v>
       </c>
       <c r="B26" s="332" t="s">
@@ -68624,7 +68644,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A27" s="330"/>
+      <c r="A27" s="331"/>
       <c r="B27" s="333"/>
       <c r="C27" s="131" t="s">
         <v>2358</v>
@@ -68637,7 +68657,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A28" s="330"/>
+      <c r="A28" s="331"/>
       <c r="B28" s="333"/>
       <c r="C28" s="131" t="s">
         <v>2360</v>
@@ -68650,7 +68670,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A29" s="330"/>
+      <c r="A29" s="331"/>
       <c r="B29" s="333"/>
       <c r="C29" s="131" t="s">
         <v>2362</v>
@@ -68663,7 +68683,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A30" s="330"/>
+      <c r="A30" s="331"/>
       <c r="B30" s="333"/>
       <c r="C30" s="131" t="s">
         <v>2364</v>
@@ -68703,10 +68723,10 @@
       <c r="D33" s="123"/>
     </row>
     <row r="34" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A34" s="329" t="s">
+      <c r="A34" s="330" t="s">
         <v>1175</v>
       </c>
-      <c r="B34" s="329" t="s">
+      <c r="B34" s="330" t="s">
         <v>2369</v>
       </c>
       <c r="C34" s="124" t="s">
@@ -68720,8 +68740,8 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A35" s="330"/>
-      <c r="B35" s="330"/>
+      <c r="A35" s="331"/>
+      <c r="B35" s="331"/>
       <c r="C35" s="124" t="s">
         <v>2372</v>
       </c>
@@ -68733,8 +68753,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A36" s="330"/>
-      <c r="B36" s="330"/>
+      <c r="A36" s="331"/>
+      <c r="B36" s="331"/>
       <c r="C36" s="124" t="s">
         <v>2374</v>
       </c>
@@ -68746,8 +68766,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A37" s="330"/>
-      <c r="B37" s="330"/>
+      <c r="A37" s="331"/>
+      <c r="B37" s="331"/>
       <c r="C37" s="124" t="s">
         <v>2376</v>
       </c>
@@ -68759,8 +68779,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A38" s="330"/>
-      <c r="B38" s="330"/>
+      <c r="A38" s="331"/>
+      <c r="B38" s="331"/>
       <c r="C38" s="124" t="s">
         <v>2378</v>
       </c>
@@ -68772,8 +68792,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A39" s="330"/>
-      <c r="B39" s="330"/>
+      <c r="A39" s="331"/>
+      <c r="B39" s="331"/>
       <c r="C39" s="124" t="s">
         <v>2380</v>
       </c>
@@ -68785,8 +68805,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A40" s="330"/>
-      <c r="B40" s="330"/>
+      <c r="A40" s="331"/>
+      <c r="B40" s="331"/>
       <c r="C40" s="124" t="s">
         <v>2382</v>
       </c>
@@ -68798,8 +68818,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A41" s="330"/>
-      <c r="B41" s="330"/>
+      <c r="A41" s="331"/>
+      <c r="B41" s="331"/>
       <c r="C41" s="124" t="s">
         <v>862</v>
       </c>
@@ -68811,8 +68831,8 @@
       </c>
     </row>
     <row r="42" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A42" s="330"/>
-      <c r="B42" s="330"/>
+      <c r="A42" s="331"/>
+      <c r="B42" s="331"/>
       <c r="C42" s="124" t="s">
         <v>2385</v>
       </c>
@@ -68824,8 +68844,8 @@
       </c>
     </row>
     <row r="43" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A43" s="330"/>
-      <c r="B43" s="330"/>
+      <c r="A43" s="331"/>
+      <c r="B43" s="331"/>
       <c r="C43" s="124" t="s">
         <v>2387</v>
       </c>
@@ -68847,7 +68867,7 @@
       <c r="D45" s="123"/>
     </row>
     <row r="46" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A46" s="329" t="s">
+      <c r="A46" s="330" t="s">
         <v>638</v>
       </c>
       <c r="B46" s="335" t="s">
@@ -68864,7 +68884,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A47" s="330"/>
+      <c r="A47" s="331"/>
       <c r="B47" s="336"/>
       <c r="C47" s="124" t="s">
         <v>2391</v>
@@ -68877,7 +68897,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A48" s="330"/>
+      <c r="A48" s="331"/>
       <c r="B48" s="337"/>
       <c r="C48" s="124" t="s">
         <v>2393</v>
@@ -68939,7 +68959,7 @@
       <c r="D53" s="123"/>
     </row>
     <row r="54" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A54" s="329" t="s">
+      <c r="A54" s="330" t="s">
         <v>2401</v>
       </c>
       <c r="B54" s="332" t="s">
@@ -68956,7 +68976,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A55" s="330"/>
+      <c r="A55" s="331"/>
       <c r="B55" s="333"/>
       <c r="C55" s="124" t="s">
         <v>2405</v>
@@ -68969,7 +68989,7 @@
       </c>
     </row>
     <row r="56" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A56" s="330"/>
+      <c r="A56" s="331"/>
       <c r="B56" s="334"/>
       <c r="C56" s="124" t="s">
         <v>2407</v>
@@ -68987,10 +69007,10 @@
       <c r="D57" s="123"/>
     </row>
     <row r="58" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A58" s="329" t="s">
+      <c r="A58" s="330" t="s">
         <v>118</v>
       </c>
-      <c r="B58" s="329" t="s">
+      <c r="B58" s="330" t="s">
         <v>118</v>
       </c>
       <c r="C58" s="124" t="s">
@@ -69004,8 +69024,8 @@
       </c>
     </row>
     <row r="59" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A59" s="330"/>
-      <c r="B59" s="330"/>
+      <c r="A59" s="331"/>
+      <c r="B59" s="331"/>
       <c r="C59" s="124" t="s">
         <v>2412</v>
       </c>
@@ -69022,10 +69042,10 @@
       <c r="D60" s="123"/>
     </row>
     <row r="61" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A61" s="329" t="s">
+      <c r="A61" s="330" t="s">
         <v>2414</v>
       </c>
-      <c r="B61" s="329" t="s">
+      <c r="B61" s="330" t="s">
         <v>2415</v>
       </c>
       <c r="C61" s="124" t="s">
@@ -69039,8 +69059,8 @@
       </c>
     </row>
     <row r="62" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A62" s="330"/>
-      <c r="B62" s="330"/>
+      <c r="A62" s="331"/>
+      <c r="B62" s="331"/>
       <c r="C62" s="124" t="s">
         <v>2418</v>
       </c>
@@ -69074,10 +69094,10 @@
       </c>
     </row>
     <row r="66" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A66" s="329" t="s">
+      <c r="A66" s="330" t="s">
         <v>2423</v>
       </c>
-      <c r="B66" s="329" t="s">
+      <c r="B66" s="330" t="s">
         <v>2424</v>
       </c>
       <c r="C66" s="124" t="s">
@@ -69091,8 +69111,8 @@
       </c>
     </row>
     <row r="67" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A67" s="330"/>
-      <c r="B67" s="330"/>
+      <c r="A67" s="331"/>
+      <c r="B67" s="331"/>
       <c r="C67" s="124" t="s">
         <v>2427</v>
       </c>
@@ -69109,10 +69129,10 @@
       <c r="D68" s="123"/>
     </row>
     <row r="69" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A69" s="329" t="s">
+      <c r="A69" s="330" t="s">
         <v>2429</v>
       </c>
-      <c r="B69" s="329" t="s">
+      <c r="B69" s="330" t="s">
         <v>2430</v>
       </c>
       <c r="C69" s="124" t="s">
@@ -69126,8 +69146,8 @@
       </c>
     </row>
     <row r="70" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A70" s="330"/>
-      <c r="B70" s="330"/>
+      <c r="A70" s="331"/>
+      <c r="B70" s="331"/>
       <c r="C70" s="124" t="s">
         <v>2433</v>
       </c>
@@ -69172,6 +69192,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="B34:B43"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
     <mergeCell ref="A66:A67"/>
     <mergeCell ref="B66:B67"/>
     <mergeCell ref="A69:A70"/>
@@ -69182,18 +69214,6 @@
     <mergeCell ref="B58:B59"/>
     <mergeCell ref="A61:A62"/>
     <mergeCell ref="B61:B62"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A34:A43"/>
-    <mergeCell ref="B34:B43"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
- Handled ballot comments for Organization
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@1408 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/ballots/2013-01 Draft/Comments-FHIR_R1_O2_2013JAN.xlsx
+++ b/ballots/2013-01 Draft/Comments-FHIR_R1_O2_2013JAN.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11265" uniqueCount="2554">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11270" uniqueCount="2554">
   <si>
     <t xml:space="preserve">BALLOT TITLE: </t>
   </si>
@@ -12413,8 +12413,23 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="11" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="10" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -12422,14 +12437,14 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -12442,12 +12457,6 @@
     <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="28" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -12473,32 +12482,23 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="11" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="10" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -12514,6 +12514,114 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="36" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="22" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="42" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -12557,114 +12665,6 @@
     <xf numFmtId="0" fontId="23" fillId="36" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="22" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="42" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="36" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -12681,6 +12681,9 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12700,9 +12703,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="56">
@@ -13095,20 +13095,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:99" ht="45.75" customHeight="1" thickTop="1">
-      <c r="A1" s="246" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="246"/>
-      <c r="C1" s="246"/>
-      <c r="D1" s="247"/>
+      <c r="A1" s="250" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="250"/>
+      <c r="C1" s="250"/>
+      <c r="D1" s="251"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="268" t="s">
+      <c r="F1" s="252" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="269"/>
-      <c r="H1" s="269"/>
-      <c r="I1" s="269"/>
-      <c r="J1" s="270"/>
+      <c r="G1" s="253"/>
+      <c r="H1" s="253"/>
+      <c r="I1" s="253"/>
+      <c r="J1" s="254"/>
       <c r="K1" s="4"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -13116,12 +13116,12 @@
       <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:99">
-      <c r="A2" s="246" t="s">
+      <c r="A2" s="250" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="246"/>
-      <c r="C2" s="246"/>
-      <c r="D2" s="247"/>
+      <c r="B2" s="250"/>
+      <c r="C2" s="250"/>
+      <c r="D2" s="251"/>
       <c r="E2" s="3"/>
       <c r="F2" s="6" t="s">
         <v>3</v>
@@ -13137,20 +13137,20 @@
       <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:99" ht="18.75" customHeight="1">
-      <c r="A3" s="263" t="s">
+      <c r="A3" s="245" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="263"/>
-      <c r="C3" s="263"/>
-      <c r="D3" s="264"/>
+      <c r="B3" s="245"/>
+      <c r="C3" s="245"/>
+      <c r="D3" s="246"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="251" t="s">
+      <c r="F3" s="255" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="252"/>
-      <c r="H3" s="252"/>
-      <c r="I3" s="252"/>
-      <c r="J3" s="253"/>
+      <c r="G3" s="256"/>
+      <c r="H3" s="256"/>
+      <c r="I3" s="256"/>
+      <c r="J3" s="257"/>
       <c r="K3" s="10"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -13158,18 +13158,18 @@
       <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:99" ht="18.75" customHeight="1">
-      <c r="A4" s="263" t="s">
+      <c r="A4" s="245" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="263"/>
-      <c r="C4" s="263"/>
-      <c r="D4" s="264"/>
+      <c r="B4" s="245"/>
+      <c r="C4" s="245"/>
+      <c r="D4" s="246"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="265"/>
-      <c r="G4" s="266"/>
-      <c r="H4" s="266"/>
-      <c r="I4" s="266"/>
-      <c r="J4" s="267"/>
+      <c r="F4" s="247"/>
+      <c r="G4" s="248"/>
+      <c r="H4" s="248"/>
+      <c r="I4" s="248"/>
+      <c r="J4" s="249"/>
       <c r="K4" s="10"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
@@ -13177,18 +13177,18 @@
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:99" ht="18.75" customHeight="1">
-      <c r="A5" s="256" t="s">
+      <c r="A5" s="258" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="256"/>
-      <c r="C5" s="256"/>
-      <c r="D5" s="257"/>
+      <c r="B5" s="258"/>
+      <c r="C5" s="258"/>
+      <c r="D5" s="259"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="251"/>
-      <c r="G5" s="252"/>
-      <c r="H5" s="252"/>
-      <c r="I5" s="252"/>
-      <c r="J5" s="253"/>
+      <c r="F5" s="255"/>
+      <c r="G5" s="256"/>
+      <c r="H5" s="256"/>
+      <c r="I5" s="256"/>
+      <c r="J5" s="257"/>
       <c r="K5" s="10"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -13196,18 +13196,18 @@
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:99" ht="29.25" customHeight="1">
-      <c r="A6" s="258" t="s">
+      <c r="A6" s="260" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="258"/>
-      <c r="C6" s="258"/>
-      <c r="D6" s="259"/>
+      <c r="B6" s="260"/>
+      <c r="C6" s="260"/>
+      <c r="D6" s="261"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="251"/>
-      <c r="G6" s="252"/>
-      <c r="H6" s="252"/>
-      <c r="I6" s="252"/>
-      <c r="J6" s="253"/>
+      <c r="F6" s="255"/>
+      <c r="G6" s="256"/>
+      <c r="H6" s="256"/>
+      <c r="I6" s="256"/>
+      <c r="J6" s="257"/>
       <c r="K6" s="10"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
@@ -13215,18 +13215,18 @@
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:99" ht="15.75" customHeight="1">
-      <c r="A7" s="246" t="s">
+      <c r="A7" s="250" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="246"/>
-      <c r="C7" s="246"/>
-      <c r="D7" s="247"/>
+      <c r="B7" s="250"/>
+      <c r="C7" s="250"/>
+      <c r="D7" s="251"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="260"/>
-      <c r="G7" s="261"/>
-      <c r="H7" s="261"/>
-      <c r="I7" s="261"/>
-      <c r="J7" s="262"/>
+      <c r="F7" s="262"/>
+      <c r="G7" s="263"/>
+      <c r="H7" s="263"/>
+      <c r="I7" s="263"/>
+      <c r="J7" s="264"/>
       <c r="K7" s="4"/>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
@@ -13236,18 +13236,18 @@
       <c r="CU7" s="16"/>
     </row>
     <row r="8" spans="1:99" ht="17.25" customHeight="1">
-      <c r="A8" s="246" t="s">
+      <c r="A8" s="250" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="246"/>
-      <c r="C8" s="246"/>
-      <c r="D8" s="247"/>
+      <c r="B8" s="250"/>
+      <c r="C8" s="250"/>
+      <c r="D8" s="251"/>
       <c r="E8" s="17"/>
-      <c r="F8" s="248"/>
-      <c r="G8" s="249"/>
-      <c r="H8" s="249"/>
-      <c r="I8" s="249"/>
-      <c r="J8" s="250"/>
+      <c r="F8" s="266"/>
+      <c r="G8" s="267"/>
+      <c r="H8" s="267"/>
+      <c r="I8" s="267"/>
+      <c r="J8" s="268"/>
       <c r="K8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
@@ -13255,18 +13255,18 @@
       <c r="P8" s="10"/>
     </row>
     <row r="9" spans="1:99" ht="62.25" customHeight="1">
-      <c r="A9" s="246" t="s">
+      <c r="A9" s="250" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="246"/>
-      <c r="C9" s="246"/>
-      <c r="D9" s="247"/>
+      <c r="B9" s="250"/>
+      <c r="C9" s="250"/>
+      <c r="D9" s="251"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="251"/>
-      <c r="G9" s="252"/>
-      <c r="H9" s="252"/>
-      <c r="I9" s="252"/>
-      <c r="J9" s="253"/>
+      <c r="F9" s="255"/>
+      <c r="G9" s="256"/>
+      <c r="H9" s="256"/>
+      <c r="I9" s="256"/>
+      <c r="J9" s="257"/>
       <c r="K9" s="18"/>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
@@ -13274,19 +13274,19 @@
       <c r="P9" s="19"/>
     </row>
     <row r="10" spans="1:99" ht="66.75" customHeight="1">
-      <c r="A10" s="254">
+      <c r="A10" s="269">
         <f>IF(Ov=Setup!C9,Disclaimer2,IF(Ov=Setup!B9,Disclaimer,IF(Ov=Setup!D9,,)))</f>
         <v>0</v>
       </c>
-      <c r="B10" s="254"/>
-      <c r="C10" s="254"/>
-      <c r="D10" s="254"/>
-      <c r="E10" s="254"/>
-      <c r="F10" s="254"/>
-      <c r="G10" s="254"/>
-      <c r="H10" s="254"/>
-      <c r="I10" s="254"/>
-      <c r="J10" s="254"/>
+      <c r="B10" s="269"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
+      <c r="H10" s="269"/>
+      <c r="I10" s="269"/>
+      <c r="J10" s="269"/>
     </row>
     <row r="11" spans="1:99" ht="30.75" customHeight="1">
       <c r="F11" s="20" t="s">
@@ -13306,12 +13306,12 @@
       <c r="F21" s="24"/>
     </row>
     <row r="23" spans="6:7" ht="114.75" customHeight="1">
-      <c r="F23" s="255"/>
-      <c r="G23" s="255"/>
+      <c r="F23" s="270"/>
+      <c r="G23" s="270"/>
     </row>
     <row r="24" spans="6:7" ht="409.5" customHeight="1">
-      <c r="F24" s="245"/>
-      <c r="G24" s="245"/>
+      <c r="F24" s="265"/>
+      <c r="G24" s="265"/>
     </row>
     <row r="25" spans="6:7">
       <c r="F25" s="25"/>
@@ -13319,6 +13319,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="A10:J10"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="F7:J7"/>
     <mergeCell ref="A4:D4"/>
     <mergeCell ref="F4:J4"/>
     <mergeCell ref="A1:D1"/>
@@ -13326,19 +13339,6 @@
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="F3:J3"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="A10:J10"/>
-    <mergeCell ref="F23:G23"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Organization You Represent" prompt="Please put the name of the HL7 member organization you represent if it is different from the name of the organization you are employed by.  " sqref="F6"/>
@@ -13365,10 +13365,10 @@
   <dimension ref="A1:AF713"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="2" topLeftCell="E197" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="J207" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G526" sqref="G526"/>
+      <selection pane="bottomRight" activeCell="T654" sqref="T654"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -26104,7 +26104,7 @@
       <c r="AE165" s="58"/>
       <c r="AF165" s="59"/>
     </row>
-    <row r="166" spans="1:32" s="60" customFormat="1" ht="38.25" customHeight="1">
+    <row r="166" spans="1:32" s="60" customFormat="1" ht="38.25" hidden="1" customHeight="1">
       <c r="A166" s="45">
         <v>164</v>
       </c>
@@ -26145,7 +26145,7 @@
         <v>82</v>
       </c>
       <c r="R166" s="52" t="s">
-        <v>2526</v>
+        <v>72</v>
       </c>
       <c r="S166" s="52" t="s">
         <v>698</v>
@@ -27056,7 +27056,7 @@
       <c r="AE177" s="58"/>
       <c r="AF177" s="59"/>
     </row>
-    <row r="178" spans="1:32" s="60" customFormat="1" ht="38.25" customHeight="1">
+    <row r="178" spans="1:32" s="60" customFormat="1" ht="38.25" hidden="1" customHeight="1">
       <c r="A178" s="45">
         <v>176</v>
       </c>
@@ -27097,7 +27097,7 @@
         <v>737</v>
       </c>
       <c r="R178" s="52" t="s">
-        <v>2526</v>
+        <v>72</v>
       </c>
       <c r="S178" s="52" t="s">
         <v>738</v>
@@ -27294,7 +27294,7 @@
       <c r="AE180" s="58"/>
       <c r="AF180" s="59"/>
     </row>
-    <row r="181" spans="1:32" s="60" customFormat="1" ht="38.25" customHeight="1">
+    <row r="181" spans="1:32" s="60" customFormat="1" ht="38.25" hidden="1" customHeight="1">
       <c r="A181" s="45">
         <v>179</v>
       </c>
@@ -27338,7 +27338,9 @@
       <c r="Q181" s="52" t="s">
         <v>749</v>
       </c>
-      <c r="R181" s="52"/>
+      <c r="R181" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S181" s="52" t="s">
         <v>750</v>
       </c>
@@ -27836,7 +27838,7 @@
       <c r="AE187" s="58"/>
       <c r="AF187" s="59"/>
     </row>
-    <row r="188" spans="1:32" s="60" customFormat="1" ht="25.5" customHeight="1">
+    <row r="188" spans="1:32" s="60" customFormat="1" ht="25.5" hidden="1" customHeight="1">
       <c r="A188" s="45">
         <v>186</v>
       </c>
@@ -27872,7 +27874,9 @@
       </c>
       <c r="P188" s="52"/>
       <c r="Q188" s="52"/>
-      <c r="R188" s="52"/>
+      <c r="R188" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S188" s="52"/>
       <c r="T188" s="53"/>
       <c r="U188" s="53"/>
@@ -27962,7 +27966,7 @@
       <c r="AE189" s="58"/>
       <c r="AF189" s="59"/>
     </row>
-    <row r="190" spans="1:32" s="60" customFormat="1" ht="25.5" customHeight="1">
+    <row r="190" spans="1:32" s="60" customFormat="1" ht="25.5" hidden="1" customHeight="1">
       <c r="A190" s="45">
         <v>188</v>
       </c>
@@ -27998,7 +28002,9 @@
       </c>
       <c r="P190" s="52"/>
       <c r="Q190" s="52"/>
-      <c r="R190" s="52"/>
+      <c r="R190" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S190" s="52"/>
       <c r="T190" s="53"/>
       <c r="U190" s="53"/>
@@ -28026,7 +28032,7 @@
       <c r="AE190" s="58"/>
       <c r="AF190" s="59"/>
     </row>
-    <row r="191" spans="1:32" s="60" customFormat="1" ht="25.5" customHeight="1">
+    <row r="191" spans="1:32" s="60" customFormat="1" ht="25.5" hidden="1" customHeight="1">
       <c r="A191" s="45">
         <v>189</v>
       </c>
@@ -28062,7 +28068,9 @@
       </c>
       <c r="P191" s="52"/>
       <c r="Q191" s="52"/>
-      <c r="R191" s="52"/>
+      <c r="R191" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S191" s="52"/>
       <c r="T191" s="53"/>
       <c r="U191" s="53"/>
@@ -28392,7 +28400,7 @@
       <c r="AE195" s="158"/>
       <c r="AF195" s="159"/>
     </row>
-    <row r="196" spans="1:32" s="60" customFormat="1" ht="25.5" customHeight="1">
+    <row r="196" spans="1:32" s="60" customFormat="1" ht="25.5" hidden="1" customHeight="1">
       <c r="A196" s="146">
         <v>194</v>
       </c>
@@ -28429,7 +28437,7 @@
       <c r="P196" s="152"/>
       <c r="Q196" s="152"/>
       <c r="R196" s="152" t="s">
-        <v>2526</v>
+        <v>72</v>
       </c>
       <c r="S196" s="152" t="s">
         <v>2529</v>
@@ -28815,7 +28823,7 @@
         <v>794</v>
       </c>
       <c r="R201" s="180" t="s">
-        <v>2526</v>
+        <v>72</v>
       </c>
       <c r="S201" s="180" t="s">
         <v>707</v>
@@ -29680,7 +29688,9 @@
       <c r="Q213" s="208" t="s">
         <v>82</v>
       </c>
-      <c r="R213" s="208"/>
+      <c r="R213" s="208" t="s">
+        <v>72</v>
+      </c>
       <c r="S213" s="208"/>
       <c r="T213" s="209"/>
       <c r="U213" s="209"/>
@@ -30402,7 +30412,7 @@
       <c r="AE223" s="58"/>
       <c r="AF223" s="59"/>
     </row>
-    <row r="224" spans="1:32" s="60" customFormat="1" ht="25.5" customHeight="1">
+    <row r="224" spans="1:32" s="60" customFormat="1" ht="25.5" hidden="1" customHeight="1">
       <c r="A224" s="45">
         <v>222</v>
       </c>
@@ -65860,10 +65870,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="13.5" customHeight="1" thickBot="1">
-      <c r="H1" s="317" t="s">
+      <c r="H1" s="278" t="s">
         <v>2237</v>
       </c>
-      <c r="I1" s="317"/>
+      <c r="I1" s="278"/>
     </row>
     <row r="2" spans="2:14" ht="15.75" customHeight="1">
       <c r="B2" s="75" t="s">
@@ -65878,16 +65888,16 @@
       <c r="I2" s="77"/>
     </row>
     <row r="3" spans="2:14" ht="303.75" customHeight="1" thickBot="1">
-      <c r="B3" s="318" t="s">
+      <c r="B3" s="279" t="s">
         <v>2239</v>
       </c>
-      <c r="C3" s="319"/>
-      <c r="D3" s="319"/>
-      <c r="E3" s="319"/>
-      <c r="F3" s="319"/>
-      <c r="G3" s="319"/>
-      <c r="H3" s="319"/>
-      <c r="I3" s="320"/>
+      <c r="C3" s="280"/>
+      <c r="D3" s="280"/>
+      <c r="E3" s="280"/>
+      <c r="F3" s="280"/>
+      <c r="G3" s="280"/>
+      <c r="H3" s="280"/>
+      <c r="I3" s="281"/>
     </row>
     <row r="4" spans="2:14" ht="13.5" customHeight="1" thickBot="1">
       <c r="J4" s="25"/>
@@ -65905,16 +65915,16 @@
       <c r="I5" s="77"/>
     </row>
     <row r="6" spans="2:14" ht="18" customHeight="1">
-      <c r="B6" s="300" t="s">
+      <c r="B6" s="282" t="s">
         <v>2241</v>
       </c>
-      <c r="C6" s="301"/>
-      <c r="D6" s="301"/>
-      <c r="E6" s="301"/>
-      <c r="F6" s="301"/>
-      <c r="G6" s="301"/>
-      <c r="H6" s="301"/>
-      <c r="I6" s="302"/>
+      <c r="C6" s="283"/>
+      <c r="D6" s="283"/>
+      <c r="E6" s="283"/>
+      <c r="F6" s="283"/>
+      <c r="G6" s="283"/>
+      <c r="H6" s="283"/>
+      <c r="I6" s="284"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -65924,15 +65934,15 @@
       <c r="B7" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="321" t="s">
+      <c r="C7" s="285" t="s">
         <v>2242</v>
       </c>
-      <c r="D7" s="322"/>
-      <c r="E7" s="322"/>
-      <c r="F7" s="322"/>
-      <c r="G7" s="322"/>
-      <c r="H7" s="322"/>
-      <c r="I7" s="323"/>
+      <c r="D7" s="286"/>
+      <c r="E7" s="286"/>
+      <c r="F7" s="286"/>
+      <c r="G7" s="286"/>
+      <c r="H7" s="286"/>
+      <c r="I7" s="287"/>
       <c r="J7" s="79"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -65942,15 +65952,15 @@
       <c r="B8" s="80" t="s">
         <v>2243</v>
       </c>
-      <c r="C8" s="324" t="s">
+      <c r="C8" s="288" t="s">
         <v>2244</v>
       </c>
-      <c r="D8" s="324"/>
-      <c r="E8" s="324"/>
-      <c r="F8" s="324"/>
-      <c r="G8" s="324"/>
-      <c r="H8" s="324"/>
-      <c r="I8" s="325"/>
+      <c r="D8" s="288"/>
+      <c r="E8" s="288"/>
+      <c r="F8" s="288"/>
+      <c r="G8" s="288"/>
+      <c r="H8" s="288"/>
+      <c r="I8" s="289"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -65960,15 +65970,15 @@
       <c r="B9" s="81" t="s">
         <v>2245</v>
       </c>
-      <c r="C9" s="315" t="s">
+      <c r="C9" s="276" t="s">
         <v>2246</v>
       </c>
-      <c r="D9" s="315"/>
-      <c r="E9" s="315"/>
-      <c r="F9" s="315"/>
-      <c r="G9" s="315"/>
-      <c r="H9" s="315"/>
-      <c r="I9" s="316"/>
+      <c r="D9" s="276"/>
+      <c r="E9" s="276"/>
+      <c r="F9" s="276"/>
+      <c r="G9" s="276"/>
+      <c r="H9" s="276"/>
+      <c r="I9" s="277"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -65979,13 +65989,13 @@
       <c r="C10" s="83" t="s">
         <v>2247</v>
       </c>
-      <c r="D10" s="313" t="s">
+      <c r="D10" s="291" t="s">
         <v>2248</v>
       </c>
       <c r="E10" s="292"/>
       <c r="F10" s="292"/>
       <c r="G10" s="292"/>
-      <c r="H10" s="314"/>
+      <c r="H10" s="293"/>
       <c r="I10" s="84"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -65997,13 +66007,13 @@
       <c r="C11" s="83" t="s">
         <v>2249</v>
       </c>
-      <c r="D11" s="313" t="s">
+      <c r="D11" s="291" t="s">
         <v>2250</v>
       </c>
       <c r="E11" s="292"/>
       <c r="F11" s="292"/>
       <c r="G11" s="292"/>
-      <c r="H11" s="314"/>
+      <c r="H11" s="293"/>
       <c r="I11" s="84"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -66016,13 +66026,13 @@
       <c r="C12" s="83" t="s">
         <v>2251</v>
       </c>
-      <c r="D12" s="313" t="s">
+      <c r="D12" s="291" t="s">
         <v>2252</v>
       </c>
       <c r="E12" s="292"/>
       <c r="F12" s="292"/>
       <c r="G12" s="292"/>
-      <c r="H12" s="314"/>
+      <c r="H12" s="293"/>
       <c r="I12" s="84"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -66034,13 +66044,13 @@
       <c r="C13" s="83" t="s">
         <v>2253</v>
       </c>
-      <c r="D13" s="313" t="s">
+      <c r="D13" s="291" t="s">
         <v>2254</v>
       </c>
       <c r="E13" s="292"/>
       <c r="F13" s="292"/>
       <c r="G13" s="292"/>
-      <c r="H13" s="314"/>
+      <c r="H13" s="293"/>
       <c r="I13" s="84"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -66052,13 +66062,13 @@
       <c r="C14" s="83" t="s">
         <v>2255</v>
       </c>
-      <c r="D14" s="313" t="s">
+      <c r="D14" s="291" t="s">
         <v>2256</v>
       </c>
       <c r="E14" s="292"/>
       <c r="F14" s="292"/>
       <c r="G14" s="292"/>
-      <c r="H14" s="314"/>
+      <c r="H14" s="293"/>
       <c r="I14" s="84"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -66070,13 +66080,13 @@
       <c r="C15" s="83" t="s">
         <v>2257</v>
       </c>
-      <c r="D15" s="313" t="s">
+      <c r="D15" s="291" t="s">
         <v>2258</v>
       </c>
       <c r="E15" s="292"/>
       <c r="F15" s="292"/>
       <c r="G15" s="292"/>
-      <c r="H15" s="314"/>
+      <c r="H15" s="293"/>
       <c r="I15" s="84"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -66088,13 +66098,13 @@
       <c r="C16" s="83" t="s">
         <v>2259</v>
       </c>
-      <c r="D16" s="313" t="s">
+      <c r="D16" s="291" t="s">
         <v>2260</v>
       </c>
       <c r="E16" s="292"/>
       <c r="F16" s="292"/>
       <c r="G16" s="292"/>
-      <c r="H16" s="314"/>
+      <c r="H16" s="293"/>
       <c r="I16" s="84"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -66106,13 +66116,13 @@
       <c r="C17" s="83" t="s">
         <v>2261</v>
       </c>
-      <c r="D17" s="313" t="s">
+      <c r="D17" s="291" t="s">
         <v>2262</v>
       </c>
       <c r="E17" s="292"/>
       <c r="F17" s="292"/>
       <c r="G17" s="292"/>
-      <c r="H17" s="314"/>
+      <c r="H17" s="293"/>
       <c r="I17" s="84"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -66124,13 +66134,13 @@
       <c r="C18" s="83" t="s">
         <v>2263</v>
       </c>
-      <c r="D18" s="313" t="s">
+      <c r="D18" s="291" t="s">
         <v>2264</v>
       </c>
       <c r="E18" s="292"/>
       <c r="F18" s="292"/>
       <c r="G18" s="292"/>
-      <c r="H18" s="314"/>
+      <c r="H18" s="293"/>
       <c r="I18" s="84"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -66155,15 +66165,15 @@
       <c r="B20" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="296" t="s">
+      <c r="C20" s="294" t="s">
         <v>2265</v>
       </c>
-      <c r="D20" s="296"/>
-      <c r="E20" s="296"/>
-      <c r="F20" s="296"/>
-      <c r="G20" s="296"/>
-      <c r="H20" s="296"/>
-      <c r="I20" s="297"/>
+      <c r="D20" s="294"/>
+      <c r="E20" s="294"/>
+      <c r="F20" s="294"/>
+      <c r="G20" s="294"/>
+      <c r="H20" s="294"/>
+      <c r="I20" s="295"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -66181,11 +66191,11 @@
       <c r="F21" s="292"/>
       <c r="G21" s="292"/>
       <c r="H21" s="292"/>
-      <c r="I21" s="293"/>
+      <c r="I21" s="296"/>
       <c r="J21" s="89"/>
-      <c r="K21" s="312"/>
-      <c r="L21" s="312"/>
-      <c r="M21" s="312"/>
+      <c r="K21" s="290"/>
+      <c r="L21" s="290"/>
+      <c r="M21" s="290"/>
     </row>
     <row r="22" spans="2:13" ht="27.75" customHeight="1">
       <c r="B22" s="80" t="s">
@@ -66199,7 +66209,7 @@
       <c r="F22" s="292"/>
       <c r="G22" s="292"/>
       <c r="H22" s="292"/>
-      <c r="I22" s="293"/>
+      <c r="I22" s="296"/>
       <c r="J22" s="89"/>
       <c r="K22" s="90"/>
       <c r="L22" s="90"/>
@@ -66209,45 +66219,45 @@
       <c r="B23" s="80" t="s">
         <v>2269</v>
       </c>
-      <c r="C23" s="294" t="s">
+      <c r="C23" s="299" t="s">
         <v>2270</v>
       </c>
-      <c r="D23" s="294"/>
-      <c r="E23" s="294"/>
-      <c r="F23" s="294"/>
-      <c r="G23" s="294"/>
-      <c r="H23" s="294"/>
-      <c r="I23" s="295"/>
+      <c r="D23" s="299"/>
+      <c r="E23" s="299"/>
+      <c r="F23" s="299"/>
+      <c r="G23" s="299"/>
+      <c r="H23" s="299"/>
+      <c r="I23" s="300"/>
       <c r="M23" s="2"/>
     </row>
     <row r="24" spans="2:13" ht="18" customHeight="1">
       <c r="B24" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="296" t="s">
+      <c r="C24" s="294" t="s">
         <v>2271</v>
       </c>
-      <c r="D24" s="296"/>
-      <c r="E24" s="296"/>
-      <c r="F24" s="296"/>
-      <c r="G24" s="296"/>
-      <c r="H24" s="296"/>
-      <c r="I24" s="297"/>
+      <c r="D24" s="294"/>
+      <c r="E24" s="294"/>
+      <c r="F24" s="294"/>
+      <c r="G24" s="294"/>
+      <c r="H24" s="294"/>
+      <c r="I24" s="295"/>
       <c r="M24" s="2"/>
     </row>
     <row r="25" spans="2:13" ht="15.75" customHeight="1">
       <c r="B25" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="296" t="s">
+      <c r="C25" s="294" t="s">
         <v>2272</v>
       </c>
-      <c r="D25" s="296"/>
-      <c r="E25" s="296"/>
-      <c r="F25" s="296"/>
-      <c r="G25" s="296"/>
-      <c r="H25" s="296"/>
-      <c r="I25" s="297"/>
+      <c r="D25" s="294"/>
+      <c r="E25" s="294"/>
+      <c r="F25" s="294"/>
+      <c r="G25" s="294"/>
+      <c r="H25" s="294"/>
+      <c r="I25" s="295"/>
       <c r="J25" s="91"/>
       <c r="M25" s="2"/>
     </row>
@@ -66255,15 +66265,15 @@
       <c r="B26" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="296" t="s">
+      <c r="C26" s="294" t="s">
         <v>2273</v>
       </c>
-      <c r="D26" s="296"/>
-      <c r="E26" s="296"/>
-      <c r="F26" s="296"/>
-      <c r="G26" s="296"/>
-      <c r="H26" s="296"/>
-      <c r="I26" s="297"/>
+      <c r="D26" s="294"/>
+      <c r="E26" s="294"/>
+      <c r="F26" s="294"/>
+      <c r="G26" s="294"/>
+      <c r="H26" s="294"/>
+      <c r="I26" s="295"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -66273,28 +66283,28 @@
       <c r="B27" s="92" t="s">
         <v>2274</v>
       </c>
-      <c r="C27" s="298" t="s">
+      <c r="C27" s="301" t="s">
         <v>2275</v>
       </c>
-      <c r="D27" s="298"/>
-      <c r="E27" s="298"/>
-      <c r="F27" s="298"/>
-      <c r="G27" s="298"/>
-      <c r="H27" s="298"/>
-      <c r="I27" s="299"/>
+      <c r="D27" s="301"/>
+      <c r="E27" s="301"/>
+      <c r="F27" s="301"/>
+      <c r="G27" s="301"/>
+      <c r="H27" s="301"/>
+      <c r="I27" s="302"/>
       <c r="J27" s="25"/>
     </row>
     <row r="28" spans="2:13" ht="18" customHeight="1">
-      <c r="B28" s="300" t="s">
+      <c r="B28" s="282" t="s">
         <v>2276</v>
       </c>
-      <c r="C28" s="301"/>
-      <c r="D28" s="301"/>
-      <c r="E28" s="301"/>
-      <c r="F28" s="301"/>
-      <c r="G28" s="301"/>
-      <c r="H28" s="301"/>
-      <c r="I28" s="302"/>
+      <c r="C28" s="283"/>
+      <c r="D28" s="283"/>
+      <c r="E28" s="283"/>
+      <c r="F28" s="283"/>
+      <c r="G28" s="283"/>
+      <c r="H28" s="283"/>
+      <c r="I28" s="284"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -66358,15 +66368,15 @@
       <c r="B32" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="290" t="s">
+      <c r="C32" s="297" t="s">
         <v>2282</v>
       </c>
-      <c r="D32" s="290"/>
-      <c r="E32" s="290"/>
-      <c r="F32" s="290"/>
-      <c r="G32" s="290"/>
-      <c r="H32" s="290"/>
-      <c r="I32" s="291"/>
+      <c r="D32" s="297"/>
+      <c r="E32" s="297"/>
+      <c r="F32" s="297"/>
+      <c r="G32" s="297"/>
+      <c r="H32" s="297"/>
+      <c r="I32" s="298"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -66376,15 +66386,15 @@
       <c r="B33" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="290" t="s">
+      <c r="C33" s="297" t="s">
         <v>2283</v>
       </c>
-      <c r="D33" s="290"/>
-      <c r="E33" s="290"/>
-      <c r="F33" s="290"/>
-      <c r="G33" s="290"/>
-      <c r="H33" s="290"/>
-      <c r="I33" s="291"/>
+      <c r="D33" s="297"/>
+      <c r="E33" s="297"/>
+      <c r="F33" s="297"/>
+      <c r="G33" s="297"/>
+      <c r="H33" s="297"/>
+      <c r="I33" s="298"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -66394,15 +66404,15 @@
       <c r="B34" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="279" t="s">
+      <c r="C34" s="315" t="s">
         <v>2284</v>
       </c>
-      <c r="D34" s="279"/>
-      <c r="E34" s="279"/>
-      <c r="F34" s="279"/>
-      <c r="G34" s="279"/>
-      <c r="H34" s="279"/>
-      <c r="I34" s="280"/>
+      <c r="D34" s="315"/>
+      <c r="E34" s="315"/>
+      <c r="F34" s="315"/>
+      <c r="G34" s="315"/>
+      <c r="H34" s="315"/>
+      <c r="I34" s="316"/>
       <c r="J34" s="2"/>
       <c r="K34" s="90"/>
       <c r="L34" s="90"/>
@@ -66412,15 +66422,15 @@
       <c r="B35" s="96" t="s">
         <v>2285</v>
       </c>
-      <c r="C35" s="279" t="s">
+      <c r="C35" s="315" t="s">
         <v>2286</v>
       </c>
-      <c r="D35" s="279"/>
-      <c r="E35" s="279"/>
-      <c r="F35" s="279"/>
-      <c r="G35" s="279"/>
-      <c r="H35" s="279"/>
-      <c r="I35" s="280"/>
+      <c r="D35" s="315"/>
+      <c r="E35" s="315"/>
+      <c r="F35" s="315"/>
+      <c r="G35" s="315"/>
+      <c r="H35" s="315"/>
+      <c r="I35" s="316"/>
       <c r="J35" s="2"/>
       <c r="K35" s="90"/>
       <c r="L35" s="90"/>
@@ -66430,15 +66440,15 @@
       <c r="B36" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="279" t="s">
+      <c r="C36" s="315" t="s">
         <v>2287</v>
       </c>
-      <c r="D36" s="279"/>
-      <c r="E36" s="279"/>
-      <c r="F36" s="279"/>
-      <c r="G36" s="279"/>
-      <c r="H36" s="279"/>
-      <c r="I36" s="280"/>
+      <c r="D36" s="315"/>
+      <c r="E36" s="315"/>
+      <c r="F36" s="315"/>
+      <c r="G36" s="315"/>
+      <c r="H36" s="315"/>
+      <c r="I36" s="316"/>
       <c r="J36" s="2"/>
       <c r="K36" s="90"/>
       <c r="L36" s="90"/>
@@ -66448,15 +66458,15 @@
       <c r="B37" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="279" t="s">
+      <c r="C37" s="315" t="s">
         <v>2288</v>
       </c>
-      <c r="D37" s="279"/>
-      <c r="E37" s="279"/>
-      <c r="F37" s="279"/>
-      <c r="G37" s="279"/>
-      <c r="H37" s="279"/>
-      <c r="I37" s="280"/>
+      <c r="D37" s="315"/>
+      <c r="E37" s="315"/>
+      <c r="F37" s="315"/>
+      <c r="G37" s="315"/>
+      <c r="H37" s="315"/>
+      <c r="I37" s="316"/>
       <c r="J37" s="2"/>
       <c r="K37" s="90"/>
       <c r="L37" s="90"/>
@@ -66466,122 +66476,140 @@
       <c r="B38" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="281" t="s">
+      <c r="C38" s="317" t="s">
         <v>2289</v>
       </c>
-      <c r="D38" s="282"/>
-      <c r="E38" s="282"/>
-      <c r="F38" s="282"/>
-      <c r="G38" s="282"/>
-      <c r="H38" s="282"/>
-      <c r="I38" s="283"/>
+      <c r="D38" s="318"/>
+      <c r="E38" s="318"/>
+      <c r="F38" s="318"/>
+      <c r="G38" s="318"/>
+      <c r="H38" s="318"/>
+      <c r="I38" s="319"/>
     </row>
     <row r="39" spans="2:13" ht="54.75" customHeight="1" thickBot="1">
       <c r="B39" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="281" t="s">
+      <c r="C39" s="317" t="s">
         <v>2290</v>
       </c>
-      <c r="D39" s="282"/>
-      <c r="E39" s="282"/>
-      <c r="F39" s="282"/>
-      <c r="G39" s="282"/>
-      <c r="H39" s="282"/>
-      <c r="I39" s="283"/>
+      <c r="D39" s="318"/>
+      <c r="E39" s="318"/>
+      <c r="F39" s="318"/>
+      <c r="G39" s="318"/>
+      <c r="H39" s="318"/>
+      <c r="I39" s="319"/>
     </row>
     <row r="40" spans="2:13" ht="40.5" customHeight="1" thickBot="1">
       <c r="B40" s="100" t="s">
         <v>2291</v>
       </c>
-      <c r="C40" s="284" t="s">
+      <c r="C40" s="320" t="s">
         <v>2292</v>
       </c>
-      <c r="D40" s="285"/>
-      <c r="E40" s="285"/>
-      <c r="F40" s="285"/>
-      <c r="G40" s="285"/>
-      <c r="H40" s="285"/>
-      <c r="I40" s="286"/>
+      <c r="D40" s="321"/>
+      <c r="E40" s="321"/>
+      <c r="F40" s="321"/>
+      <c r="G40" s="321"/>
+      <c r="H40" s="321"/>
+      <c r="I40" s="322"/>
     </row>
     <row r="41" spans="2:13" ht="40.5" customHeight="1" thickBot="1">
       <c r="B41" s="101" t="s">
         <v>2293</v>
       </c>
-      <c r="C41" s="287" t="s">
+      <c r="C41" s="323" t="s">
         <v>2294</v>
       </c>
-      <c r="D41" s="285"/>
-      <c r="E41" s="285"/>
-      <c r="F41" s="285"/>
-      <c r="G41" s="285"/>
-      <c r="H41" s="285"/>
-      <c r="I41" s="286"/>
+      <c r="D41" s="321"/>
+      <c r="E41" s="321"/>
+      <c r="F41" s="321"/>
+      <c r="G41" s="321"/>
+      <c r="H41" s="321"/>
+      <c r="I41" s="322"/>
     </row>
     <row r="42" spans="2:13" ht="40.5" customHeight="1" thickBot="1">
       <c r="B42" s="102" t="s">
         <v>2295</v>
       </c>
-      <c r="C42" s="288" t="s">
+      <c r="C42" s="324" t="s">
         <v>2296</v>
       </c>
-      <c r="D42" s="288"/>
-      <c r="E42" s="288"/>
-      <c r="F42" s="288"/>
-      <c r="G42" s="288"/>
-      <c r="H42" s="288"/>
-      <c r="I42" s="289"/>
+      <c r="D42" s="324"/>
+      <c r="E42" s="324"/>
+      <c r="F42" s="324"/>
+      <c r="G42" s="324"/>
+      <c r="H42" s="324"/>
+      <c r="I42" s="325"/>
     </row>
     <row r="43" spans="2:13" ht="43.5" customHeight="1" thickBot="1">
       <c r="B43" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="276" t="s">
+      <c r="C43" s="312" t="s">
         <v>2297</v>
       </c>
-      <c r="D43" s="277"/>
-      <c r="E43" s="277"/>
-      <c r="F43" s="277"/>
-      <c r="G43" s="277"/>
-      <c r="H43" s="277"/>
-      <c r="I43" s="278"/>
+      <c r="D43" s="313"/>
+      <c r="E43" s="313"/>
+      <c r="F43" s="313"/>
+      <c r="G43" s="313"/>
+      <c r="H43" s="313"/>
+      <c r="I43" s="314"/>
     </row>
     <row r="44" spans="2:13" ht="13.5" customHeight="1" thickBot="1">
       <c r="B44" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="276" t="s">
+      <c r="C44" s="312" t="s">
         <v>2298</v>
       </c>
-      <c r="D44" s="277"/>
-      <c r="E44" s="277"/>
-      <c r="F44" s="277"/>
-      <c r="G44" s="277"/>
-      <c r="H44" s="277"/>
-      <c r="I44" s="278"/>
+      <c r="D44" s="313"/>
+      <c r="E44" s="313"/>
+      <c r="F44" s="313"/>
+      <c r="G44" s="313"/>
+      <c r="H44" s="313"/>
+      <c r="I44" s="314"/>
     </row>
     <row r="45" spans="2:13" ht="32.25" customHeight="1" thickBot="1">
       <c r="B45" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="276" t="s">
+      <c r="C45" s="312" t="s">
         <v>2299</v>
       </c>
-      <c r="D45" s="277"/>
-      <c r="E45" s="277"/>
-      <c r="F45" s="277"/>
-      <c r="G45" s="277"/>
-      <c r="H45" s="277"/>
-      <c r="I45" s="278"/>
+      <c r="D45" s="313"/>
+      <c r="E45" s="313"/>
+      <c r="F45" s="313"/>
+      <c r="G45" s="313"/>
+      <c r="H45" s="313"/>
+      <c r="I45" s="314"/>
     </row>
   </sheetData>
   <mergeCells count="42">
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="C45:I45"/>
+    <mergeCell ref="C34:I34"/>
+    <mergeCell ref="C35:I35"/>
+    <mergeCell ref="C36:I36"/>
+    <mergeCell ref="C37:I37"/>
+    <mergeCell ref="C38:I38"/>
+    <mergeCell ref="C39:I39"/>
+    <mergeCell ref="C40:I40"/>
+    <mergeCell ref="C41:I41"/>
+    <mergeCell ref="C42:I42"/>
+    <mergeCell ref="C43:I43"/>
+    <mergeCell ref="C44:I44"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
     <mergeCell ref="K21:M21"/>
     <mergeCell ref="D10:H10"/>
     <mergeCell ref="D11:H11"/>
@@ -66594,30 +66622,12 @@
     <mergeCell ref="D18:H18"/>
     <mergeCell ref="C20:I20"/>
     <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="C45:I45"/>
-    <mergeCell ref="C34:I34"/>
-    <mergeCell ref="C35:I35"/>
-    <mergeCell ref="C36:I36"/>
-    <mergeCell ref="C37:I37"/>
-    <mergeCell ref="C38:I38"/>
-    <mergeCell ref="C39:I39"/>
-    <mergeCell ref="C40:I40"/>
-    <mergeCell ref="C41:I41"/>
-    <mergeCell ref="C42:I42"/>
-    <mergeCell ref="C43:I43"/>
-    <mergeCell ref="C44:I44"/>
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C8:I8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H1" location="Ballot!A1" display="Ballot!A1"/>
@@ -68357,7 +68367,7 @@
       <c r="A3" s="330" t="s">
         <v>2308</v>
       </c>
-      <c r="B3" s="332" t="s">
+      <c r="B3" s="333" t="s">
         <v>2309</v>
       </c>
       <c r="C3" s="124" t="s">
@@ -68372,7 +68382,7 @@
     </row>
     <row r="4" spans="1:5" ht="28.5" customHeight="1">
       <c r="A4" s="331"/>
-      <c r="B4" s="333"/>
+      <c r="B4" s="334"/>
       <c r="C4" s="124" t="s">
         <v>2313</v>
       </c>
@@ -68385,7 +68395,7 @@
     </row>
     <row r="5" spans="1:5" ht="28.5" customHeight="1">
       <c r="A5" s="331"/>
-      <c r="B5" s="333"/>
+      <c r="B5" s="334"/>
       <c r="C5" s="124" t="s">
         <v>2316</v>
       </c>
@@ -68398,7 +68408,7 @@
     </row>
     <row r="6" spans="1:5" ht="14.25" customHeight="1">
       <c r="A6" s="331"/>
-      <c r="B6" s="333"/>
+      <c r="B6" s="334"/>
       <c r="C6" s="124" t="s">
         <v>2318</v>
       </c>
@@ -68411,7 +68421,7 @@
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1">
       <c r="A7" s="331"/>
-      <c r="B7" s="333"/>
+      <c r="B7" s="334"/>
       <c r="C7" s="124" t="s">
         <v>2257</v>
       </c>
@@ -68424,7 +68434,7 @@
     </row>
     <row r="8" spans="1:5" ht="14.25" customHeight="1">
       <c r="A8" s="331"/>
-      <c r="B8" s="333"/>
+      <c r="B8" s="334"/>
       <c r="C8" s="124" t="s">
         <v>2321</v>
       </c>
@@ -68437,7 +68447,7 @@
     </row>
     <row r="9" spans="1:5" ht="28.5" customHeight="1">
       <c r="A9" s="331"/>
-      <c r="B9" s="333"/>
+      <c r="B9" s="334"/>
       <c r="C9" s="124" t="s">
         <v>2324</v>
       </c>
@@ -68450,7 +68460,7 @@
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1">
       <c r="A10" s="331"/>
-      <c r="B10" s="333"/>
+      <c r="B10" s="334"/>
       <c r="C10" s="124" t="s">
         <v>2326</v>
       </c>
@@ -68462,8 +68472,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A11" s="338"/>
-      <c r="B11" s="334"/>
+      <c r="A11" s="332"/>
+      <c r="B11" s="335"/>
       <c r="C11" s="124" t="s">
         <v>2329</v>
       </c>
@@ -68630,7 +68640,7 @@
       <c r="A26" s="330" t="s">
         <v>2354</v>
       </c>
-      <c r="B26" s="332" t="s">
+      <c r="B26" s="333" t="s">
         <v>2355</v>
       </c>
       <c r="C26" s="124" t="s">
@@ -68645,7 +68655,7 @@
     </row>
     <row r="27" spans="1:5" ht="14.25" customHeight="1">
       <c r="A27" s="331"/>
-      <c r="B27" s="333"/>
+      <c r="B27" s="334"/>
       <c r="C27" s="131" t="s">
         <v>2358</v>
       </c>
@@ -68658,7 +68668,7 @@
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="331"/>
-      <c r="B28" s="333"/>
+      <c r="B28" s="334"/>
       <c r="C28" s="131" t="s">
         <v>2360</v>
       </c>
@@ -68671,7 +68681,7 @@
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="331"/>
-      <c r="B29" s="333"/>
+      <c r="B29" s="334"/>
       <c r="C29" s="131" t="s">
         <v>2362</v>
       </c>
@@ -68684,7 +68694,7 @@
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1">
       <c r="A30" s="331"/>
-      <c r="B30" s="333"/>
+      <c r="B30" s="334"/>
       <c r="C30" s="131" t="s">
         <v>2364</v>
       </c>
@@ -68870,7 +68880,7 @@
       <c r="A46" s="330" t="s">
         <v>638</v>
       </c>
-      <c r="B46" s="335" t="s">
+      <c r="B46" s="336" t="s">
         <v>2389</v>
       </c>
       <c r="C46" s="124" t="s">
@@ -68885,7 +68895,7 @@
     </row>
     <row r="47" spans="1:5" ht="14.25" customHeight="1">
       <c r="A47" s="331"/>
-      <c r="B47" s="336"/>
+      <c r="B47" s="337"/>
       <c r="C47" s="124" t="s">
         <v>2391</v>
       </c>
@@ -68898,7 +68908,7 @@
     </row>
     <row r="48" spans="1:5" ht="14.25" customHeight="1">
       <c r="A48" s="331"/>
-      <c r="B48" s="337"/>
+      <c r="B48" s="338"/>
       <c r="C48" s="124" t="s">
         <v>2393</v>
       </c>
@@ -68962,7 +68972,7 @@
       <c r="A54" s="330" t="s">
         <v>2401</v>
       </c>
-      <c r="B54" s="332" t="s">
+      <c r="B54" s="333" t="s">
         <v>2402</v>
       </c>
       <c r="C54" s="124" t="s">
@@ -68977,7 +68987,7 @@
     </row>
     <row r="55" spans="1:5" ht="14.25" customHeight="1">
       <c r="A55" s="331"/>
-      <c r="B55" s="333"/>
+      <c r="B55" s="334"/>
       <c r="C55" s="124" t="s">
         <v>2405</v>
       </c>
@@ -68990,7 +69000,7 @@
     </row>
     <row r="56" spans="1:5" ht="14.25" customHeight="1">
       <c r="A56" s="331"/>
-      <c r="B56" s="334"/>
+      <c r="B56" s="335"/>
       <c r="C56" s="124" t="s">
         <v>2407</v>
       </c>
@@ -69192,18 +69202,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A34:A43"/>
-    <mergeCell ref="B34:B43"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
     <mergeCell ref="A66:A67"/>
     <mergeCell ref="B66:B67"/>
     <mergeCell ref="A69:A70"/>
@@ -69214,6 +69212,18 @@
     <mergeCell ref="B58:B59"/>
     <mergeCell ref="A61:A62"/>
     <mergeCell ref="B61:B62"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="B34:B43"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
- Questionnaire draft comments handled - Questionnaire redesign - Questionnaire Extensions for validation
git-svn-id: http://gforge.hl7.org/svn/fhir/trunk@1497 2f0db536-2c49-4257-a3fa-e771ed206c19
</commit_message>
<xml_diff>
--- a/ballots/2013-01 Draft/Comments-FHIR_R1_O2_2013JAN.xlsx
+++ b/ballots/2013-01 Draft/Comments-FHIR_R1_O2_2013JAN.xlsx
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11306" uniqueCount="2556">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11308" uniqueCount="2556">
   <si>
     <t xml:space="preserve">BALLOT TITLE: </t>
   </si>
@@ -12419,23 +12419,8 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="11" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="34" borderId="10" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
@@ -12443,14 +12428,14 @@
     <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
@@ -12463,6 +12448,12 @@
     <xf numFmtId="49" fontId="0" fillId="34" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -12488,23 +12479,32 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="19" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="11" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="10" xfId="42" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="28" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -12520,114 +12520,6 @@
     </xf>
     <xf numFmtId="0" fontId="22" fillId="36" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="36" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="37" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="37" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="22" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="42" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="54" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -12671,6 +12563,114 @@
     <xf numFmtId="0" fontId="23" fillId="36" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="37" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="36" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="22" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="11" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="42" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="36" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="37" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="36" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -12687,9 +12687,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -12709,6 +12706,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="56">
@@ -13101,20 +13101,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:99" ht="45.75" customHeight="1" thickTop="1">
-      <c r="A1" s="250" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="250"/>
-      <c r="C1" s="250"/>
-      <c r="D1" s="251"/>
+      <c r="A1" s="246" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="246"/>
+      <c r="C1" s="246"/>
+      <c r="D1" s="247"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="252" t="s">
+      <c r="F1" s="268" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="253"/>
-      <c r="H1" s="253"/>
-      <c r="I1" s="253"/>
-      <c r="J1" s="254"/>
+      <c r="G1" s="269"/>
+      <c r="H1" s="269"/>
+      <c r="I1" s="269"/>
+      <c r="J1" s="270"/>
       <c r="K1" s="4"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
@@ -13122,12 +13122,12 @@
       <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:99">
-      <c r="A2" s="250" t="s">
+      <c r="A2" s="246" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="250"/>
-      <c r="C2" s="250"/>
-      <c r="D2" s="251"/>
+      <c r="B2" s="246"/>
+      <c r="C2" s="246"/>
+      <c r="D2" s="247"/>
       <c r="E2" s="3"/>
       <c r="F2" s="6" t="s">
         <v>3</v>
@@ -13143,20 +13143,20 @@
       <c r="P2" s="5"/>
     </row>
     <row r="3" spans="1:99" ht="18.75" customHeight="1">
-      <c r="A3" s="245" t="s">
+      <c r="A3" s="263" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="245"/>
-      <c r="C3" s="245"/>
-      <c r="D3" s="246"/>
+      <c r="B3" s="263"/>
+      <c r="C3" s="263"/>
+      <c r="D3" s="264"/>
       <c r="E3" s="9"/>
-      <c r="F3" s="255" t="s">
+      <c r="F3" s="251" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="256"/>
-      <c r="H3" s="256"/>
-      <c r="I3" s="256"/>
-      <c r="J3" s="257"/>
+      <c r="G3" s="252"/>
+      <c r="H3" s="252"/>
+      <c r="I3" s="252"/>
+      <c r="J3" s="253"/>
       <c r="K3" s="10"/>
       <c r="M3" s="5"/>
       <c r="N3" s="5"/>
@@ -13164,18 +13164,18 @@
       <c r="P3" s="5"/>
     </row>
     <row r="4" spans="1:99" ht="18.75" customHeight="1">
-      <c r="A4" s="245" t="s">
+      <c r="A4" s="263" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="245"/>
-      <c r="C4" s="245"/>
-      <c r="D4" s="246"/>
+      <c r="B4" s="263"/>
+      <c r="C4" s="263"/>
+      <c r="D4" s="264"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="247"/>
-      <c r="G4" s="248"/>
-      <c r="H4" s="248"/>
-      <c r="I4" s="248"/>
-      <c r="J4" s="249"/>
+      <c r="F4" s="265"/>
+      <c r="G4" s="266"/>
+      <c r="H4" s="266"/>
+      <c r="I4" s="266"/>
+      <c r="J4" s="267"/>
       <c r="K4" s="10"/>
       <c r="M4" s="5"/>
       <c r="N4" s="5"/>
@@ -13183,18 +13183,18 @@
       <c r="P4" s="5"/>
     </row>
     <row r="5" spans="1:99" ht="18.75" customHeight="1">
-      <c r="A5" s="258" t="s">
+      <c r="A5" s="256" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="258"/>
-      <c r="C5" s="258"/>
-      <c r="D5" s="259"/>
+      <c r="B5" s="256"/>
+      <c r="C5" s="256"/>
+      <c r="D5" s="257"/>
       <c r="E5" s="12"/>
-      <c r="F5" s="255"/>
-      <c r="G5" s="256"/>
-      <c r="H5" s="256"/>
-      <c r="I5" s="256"/>
-      <c r="J5" s="257"/>
+      <c r="F5" s="251"/>
+      <c r="G5" s="252"/>
+      <c r="H5" s="252"/>
+      <c r="I5" s="252"/>
+      <c r="J5" s="253"/>
       <c r="K5" s="10"/>
       <c r="M5" s="5"/>
       <c r="N5" s="5"/>
@@ -13202,18 +13202,18 @@
       <c r="P5" s="5"/>
     </row>
     <row r="6" spans="1:99" ht="29.25" customHeight="1">
-      <c r="A6" s="260" t="s">
+      <c r="A6" s="258" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="260"/>
-      <c r="C6" s="260"/>
-      <c r="D6" s="261"/>
+      <c r="B6" s="258"/>
+      <c r="C6" s="258"/>
+      <c r="D6" s="259"/>
       <c r="E6" s="13"/>
-      <c r="F6" s="255"/>
-      <c r="G6" s="256"/>
-      <c r="H6" s="256"/>
-      <c r="I6" s="256"/>
-      <c r="J6" s="257"/>
+      <c r="F6" s="251"/>
+      <c r="G6" s="252"/>
+      <c r="H6" s="252"/>
+      <c r="I6" s="252"/>
+      <c r="J6" s="253"/>
       <c r="K6" s="10"/>
       <c r="M6" s="5"/>
       <c r="N6" s="5"/>
@@ -13221,18 +13221,18 @@
       <c r="P6" s="5"/>
     </row>
     <row r="7" spans="1:99" ht="15.75" customHeight="1">
-      <c r="A7" s="250" t="s">
+      <c r="A7" s="246" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="250"/>
-      <c r="C7" s="250"/>
-      <c r="D7" s="251"/>
+      <c r="B7" s="246"/>
+      <c r="C7" s="246"/>
+      <c r="D7" s="247"/>
       <c r="E7" s="14"/>
-      <c r="F7" s="262"/>
-      <c r="G7" s="263"/>
-      <c r="H7" s="263"/>
-      <c r="I7" s="263"/>
-      <c r="J7" s="264"/>
+      <c r="F7" s="260"/>
+      <c r="G7" s="261"/>
+      <c r="H7" s="261"/>
+      <c r="I7" s="261"/>
+      <c r="J7" s="262"/>
       <c r="K7" s="4"/>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
@@ -13242,18 +13242,18 @@
       <c r="CU7" s="16"/>
     </row>
     <row r="8" spans="1:99" ht="17.25" customHeight="1">
-      <c r="A8" s="250" t="s">
+      <c r="A8" s="246" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="250"/>
-      <c r="C8" s="250"/>
-      <c r="D8" s="251"/>
+      <c r="B8" s="246"/>
+      <c r="C8" s="246"/>
+      <c r="D8" s="247"/>
       <c r="E8" s="17"/>
-      <c r="F8" s="266"/>
-      <c r="G8" s="267"/>
-      <c r="H8" s="267"/>
-      <c r="I8" s="267"/>
-      <c r="J8" s="268"/>
+      <c r="F8" s="248"/>
+      <c r="G8" s="249"/>
+      <c r="H8" s="249"/>
+      <c r="I8" s="249"/>
+      <c r="J8" s="250"/>
       <c r="K8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
@@ -13261,18 +13261,18 @@
       <c r="P8" s="10"/>
     </row>
     <row r="9" spans="1:99" ht="62.25" customHeight="1">
-      <c r="A9" s="250" t="s">
+      <c r="A9" s="246" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="250"/>
-      <c r="C9" s="250"/>
-      <c r="D9" s="251"/>
+      <c r="B9" s="246"/>
+      <c r="C9" s="246"/>
+      <c r="D9" s="247"/>
       <c r="E9" s="14"/>
-      <c r="F9" s="255"/>
-      <c r="G9" s="256"/>
-      <c r="H9" s="256"/>
-      <c r="I9" s="256"/>
-      <c r="J9" s="257"/>
+      <c r="F9" s="251"/>
+      <c r="G9" s="252"/>
+      <c r="H9" s="252"/>
+      <c r="I9" s="252"/>
+      <c r="J9" s="253"/>
       <c r="K9" s="18"/>
       <c r="M9" s="19"/>
       <c r="N9" s="19"/>
@@ -13280,19 +13280,19 @@
       <c r="P9" s="19"/>
     </row>
     <row r="10" spans="1:99" ht="66.75" customHeight="1">
-      <c r="A10" s="269">
+      <c r="A10" s="254">
         <f>IF(Ov=Setup!C9,Disclaimer2,IF(Ov=Setup!B9,Disclaimer,IF(Ov=Setup!D9,,)))</f>
         <v>0</v>
       </c>
-      <c r="B10" s="269"/>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
-      <c r="H10" s="269"/>
-      <c r="I10" s="269"/>
-      <c r="J10" s="269"/>
+      <c r="B10" s="254"/>
+      <c r="C10" s="254"/>
+      <c r="D10" s="254"/>
+      <c r="E10" s="254"/>
+      <c r="F10" s="254"/>
+      <c r="G10" s="254"/>
+      <c r="H10" s="254"/>
+      <c r="I10" s="254"/>
+      <c r="J10" s="254"/>
     </row>
     <row r="11" spans="1:99" ht="30.75" customHeight="1">
       <c r="F11" s="20" t="s">
@@ -13312,12 +13312,12 @@
       <c r="F21" s="24"/>
     </row>
     <row r="23" spans="6:7" ht="114.75" customHeight="1">
-      <c r="F23" s="270"/>
-      <c r="G23" s="270"/>
+      <c r="F23" s="255"/>
+      <c r="G23" s="255"/>
     </row>
     <row r="24" spans="6:7" ht="409.5" customHeight="1">
-      <c r="F24" s="265"/>
-      <c r="G24" s="265"/>
+      <c r="F24" s="245"/>
+      <c r="G24" s="245"/>
     </row>
     <row r="25" spans="6:7">
       <c r="F25" s="25"/>
@@ -13325,6 +13325,19 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="F4:J4"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="F3:J3"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="F7:J7"/>
     <mergeCell ref="F24:G24"/>
     <mergeCell ref="A8:D8"/>
     <mergeCell ref="F8:J8"/>
@@ -13332,19 +13345,6 @@
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="A10:J10"/>
     <mergeCell ref="F23:G23"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="F4:J4"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="F3:J3"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Organization You Represent" prompt="Please put the name of the HL7 member organization you represent if it is different from the name of the organization you are employed by.  " sqref="F6"/>
@@ -13374,7 +13374,7 @@
       <pane xSplit="4" ySplit="2" topLeftCell="E197" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F219" sqref="F219"/>
+      <selection pane="bottomRight" activeCell="A220" sqref="A220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75"/>
@@ -51542,7 +51542,9 @@
       <c r="Q523" s="52" t="s">
         <v>1616</v>
       </c>
-      <c r="R523" s="52"/>
+      <c r="R523" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S523" s="52"/>
       <c r="T523" s="53"/>
       <c r="U523" s="53"/>
@@ -51738,7 +51740,9 @@
       <c r="Q526" s="52" t="s">
         <v>1625</v>
       </c>
-      <c r="R526" s="52"/>
+      <c r="R526" s="52" t="s">
+        <v>72</v>
+      </c>
       <c r="S526" s="52"/>
       <c r="T526" s="53"/>
       <c r="U526" s="53"/>
@@ -65234,7 +65238,7 @@
       </filters>
     </filterColumn>
     <filterColumn colId="17">
-      <filters blank="1">
+      <filters>
         <filter val="N"/>
       </filters>
     </filterColumn>
@@ -65948,10 +65952,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="13.5" customHeight="1" thickBot="1">
-      <c r="H1" s="278" t="s">
+      <c r="H1" s="317" t="s">
         <v>2234</v>
       </c>
-      <c r="I1" s="278"/>
+      <c r="I1" s="317"/>
     </row>
     <row r="2" spans="2:14" ht="15.75" customHeight="1">
       <c r="B2" s="75" t="s">
@@ -65966,16 +65970,16 @@
       <c r="I2" s="77"/>
     </row>
     <row r="3" spans="2:14" ht="303.75" customHeight="1" thickBot="1">
-      <c r="B3" s="279" t="s">
+      <c r="B3" s="318" t="s">
         <v>2236</v>
       </c>
-      <c r="C3" s="280"/>
-      <c r="D3" s="280"/>
-      <c r="E3" s="280"/>
-      <c r="F3" s="280"/>
-      <c r="G3" s="280"/>
-      <c r="H3" s="280"/>
-      <c r="I3" s="281"/>
+      <c r="C3" s="319"/>
+      <c r="D3" s="319"/>
+      <c r="E3" s="319"/>
+      <c r="F3" s="319"/>
+      <c r="G3" s="319"/>
+      <c r="H3" s="319"/>
+      <c r="I3" s="320"/>
     </row>
     <row r="4" spans="2:14" ht="13.5" customHeight="1" thickBot="1">
       <c r="J4" s="25"/>
@@ -65993,16 +65997,16 @@
       <c r="I5" s="77"/>
     </row>
     <row r="6" spans="2:14" ht="18" customHeight="1">
-      <c r="B6" s="282" t="s">
+      <c r="B6" s="300" t="s">
         <v>2238</v>
       </c>
-      <c r="C6" s="283"/>
-      <c r="D6" s="283"/>
-      <c r="E6" s="283"/>
-      <c r="F6" s="283"/>
-      <c r="G6" s="283"/>
-      <c r="H6" s="283"/>
-      <c r="I6" s="284"/>
+      <c r="C6" s="301"/>
+      <c r="D6" s="301"/>
+      <c r="E6" s="301"/>
+      <c r="F6" s="301"/>
+      <c r="G6" s="301"/>
+      <c r="H6" s="301"/>
+      <c r="I6" s="302"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -66012,15 +66016,15 @@
       <c r="B7" s="78" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="285" t="s">
+      <c r="C7" s="321" t="s">
         <v>2239</v>
       </c>
-      <c r="D7" s="286"/>
-      <c r="E7" s="286"/>
-      <c r="F7" s="286"/>
-      <c r="G7" s="286"/>
-      <c r="H7" s="286"/>
-      <c r="I7" s="287"/>
+      <c r="D7" s="322"/>
+      <c r="E7" s="322"/>
+      <c r="F7" s="322"/>
+      <c r="G7" s="322"/>
+      <c r="H7" s="322"/>
+      <c r="I7" s="323"/>
       <c r="J7" s="79"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -66030,15 +66034,15 @@
       <c r="B8" s="80" t="s">
         <v>2240</v>
       </c>
-      <c r="C8" s="288" t="s">
+      <c r="C8" s="324" t="s">
         <v>2241</v>
       </c>
-      <c r="D8" s="288"/>
-      <c r="E8" s="288"/>
-      <c r="F8" s="288"/>
-      <c r="G8" s="288"/>
-      <c r="H8" s="288"/>
-      <c r="I8" s="289"/>
+      <c r="D8" s="324"/>
+      <c r="E8" s="324"/>
+      <c r="F8" s="324"/>
+      <c r="G8" s="324"/>
+      <c r="H8" s="324"/>
+      <c r="I8" s="325"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -66048,15 +66052,15 @@
       <c r="B9" s="81" t="s">
         <v>2242</v>
       </c>
-      <c r="C9" s="276" t="s">
+      <c r="C9" s="315" t="s">
         <v>2243</v>
       </c>
-      <c r="D9" s="276"/>
-      <c r="E9" s="276"/>
-      <c r="F9" s="276"/>
-      <c r="G9" s="276"/>
-      <c r="H9" s="276"/>
-      <c r="I9" s="277"/>
+      <c r="D9" s="315"/>
+      <c r="E9" s="315"/>
+      <c r="F9" s="315"/>
+      <c r="G9" s="315"/>
+      <c r="H9" s="315"/>
+      <c r="I9" s="316"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -66067,13 +66071,13 @@
       <c r="C10" s="83" t="s">
         <v>2244</v>
       </c>
-      <c r="D10" s="291" t="s">
+      <c r="D10" s="313" t="s">
         <v>2245</v>
       </c>
       <c r="E10" s="292"/>
       <c r="F10" s="292"/>
       <c r="G10" s="292"/>
-      <c r="H10" s="293"/>
+      <c r="H10" s="314"/>
       <c r="I10" s="84"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -66085,13 +66089,13 @@
       <c r="C11" s="83" t="s">
         <v>2246</v>
       </c>
-      <c r="D11" s="291" t="s">
+      <c r="D11" s="313" t="s">
         <v>2247</v>
       </c>
       <c r="E11" s="292"/>
       <c r="F11" s="292"/>
       <c r="G11" s="292"/>
-      <c r="H11" s="293"/>
+      <c r="H11" s="314"/>
       <c r="I11" s="84"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
@@ -66104,13 +66108,13 @@
       <c r="C12" s="83" t="s">
         <v>2248</v>
       </c>
-      <c r="D12" s="291" t="s">
+      <c r="D12" s="313" t="s">
         <v>2249</v>
       </c>
       <c r="E12" s="292"/>
       <c r="F12" s="292"/>
       <c r="G12" s="292"/>
-      <c r="H12" s="293"/>
+      <c r="H12" s="314"/>
       <c r="I12" s="84"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -66122,13 +66126,13 @@
       <c r="C13" s="83" t="s">
         <v>2250</v>
       </c>
-      <c r="D13" s="291" t="s">
+      <c r="D13" s="313" t="s">
         <v>2251</v>
       </c>
       <c r="E13" s="292"/>
       <c r="F13" s="292"/>
       <c r="G13" s="292"/>
-      <c r="H13" s="293"/>
+      <c r="H13" s="314"/>
       <c r="I13" s="84"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
@@ -66140,13 +66144,13 @@
       <c r="C14" s="83" t="s">
         <v>2252</v>
       </c>
-      <c r="D14" s="291" t="s">
+      <c r="D14" s="313" t="s">
         <v>2253</v>
       </c>
       <c r="E14" s="292"/>
       <c r="F14" s="292"/>
       <c r="G14" s="292"/>
-      <c r="H14" s="293"/>
+      <c r="H14" s="314"/>
       <c r="I14" s="84"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -66158,13 +66162,13 @@
       <c r="C15" s="83" t="s">
         <v>2254</v>
       </c>
-      <c r="D15" s="291" t="s">
+      <c r="D15" s="313" t="s">
         <v>2255</v>
       </c>
       <c r="E15" s="292"/>
       <c r="F15" s="292"/>
       <c r="G15" s="292"/>
-      <c r="H15" s="293"/>
+      <c r="H15" s="314"/>
       <c r="I15" s="84"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
@@ -66176,13 +66180,13 @@
       <c r="C16" s="83" t="s">
         <v>2256</v>
       </c>
-      <c r="D16" s="291" t="s">
+      <c r="D16" s="313" t="s">
         <v>2257</v>
       </c>
       <c r="E16" s="292"/>
       <c r="F16" s="292"/>
       <c r="G16" s="292"/>
-      <c r="H16" s="293"/>
+      <c r="H16" s="314"/>
       <c r="I16" s="84"/>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -66194,13 +66198,13 @@
       <c r="C17" s="83" t="s">
         <v>2258</v>
       </c>
-      <c r="D17" s="291" t="s">
+      <c r="D17" s="313" t="s">
         <v>2259</v>
       </c>
       <c r="E17" s="292"/>
       <c r="F17" s="292"/>
       <c r="G17" s="292"/>
-      <c r="H17" s="293"/>
+      <c r="H17" s="314"/>
       <c r="I17" s="84"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
@@ -66212,13 +66216,13 @@
       <c r="C18" s="83" t="s">
         <v>2260</v>
       </c>
-      <c r="D18" s="291" t="s">
+      <c r="D18" s="313" t="s">
         <v>2261</v>
       </c>
       <c r="E18" s="292"/>
       <c r="F18" s="292"/>
       <c r="G18" s="292"/>
-      <c r="H18" s="293"/>
+      <c r="H18" s="314"/>
       <c r="I18" s="84"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -66243,15 +66247,15 @@
       <c r="B20" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="294" t="s">
+      <c r="C20" s="296" t="s">
         <v>2262</v>
       </c>
-      <c r="D20" s="294"/>
-      <c r="E20" s="294"/>
-      <c r="F20" s="294"/>
-      <c r="G20" s="294"/>
-      <c r="H20" s="294"/>
-      <c r="I20" s="295"/>
+      <c r="D20" s="296"/>
+      <c r="E20" s="296"/>
+      <c r="F20" s="296"/>
+      <c r="G20" s="296"/>
+      <c r="H20" s="296"/>
+      <c r="I20" s="297"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -66269,11 +66273,11 @@
       <c r="F21" s="292"/>
       <c r="G21" s="292"/>
       <c r="H21" s="292"/>
-      <c r="I21" s="296"/>
+      <c r="I21" s="293"/>
       <c r="J21" s="89"/>
-      <c r="K21" s="290"/>
-      <c r="L21" s="290"/>
-      <c r="M21" s="290"/>
+      <c r="K21" s="312"/>
+      <c r="L21" s="312"/>
+      <c r="M21" s="312"/>
     </row>
     <row r="22" spans="2:13" ht="27.75" customHeight="1">
       <c r="B22" s="80" t="s">
@@ -66287,7 +66291,7 @@
       <c r="F22" s="292"/>
       <c r="G22" s="292"/>
       <c r="H22" s="292"/>
-      <c r="I22" s="296"/>
+      <c r="I22" s="293"/>
       <c r="J22" s="89"/>
       <c r="K22" s="90"/>
       <c r="L22" s="90"/>
@@ -66297,45 +66301,45 @@
       <c r="B23" s="80" t="s">
         <v>2266</v>
       </c>
-      <c r="C23" s="299" t="s">
+      <c r="C23" s="294" t="s">
         <v>2267</v>
       </c>
-      <c r="D23" s="299"/>
-      <c r="E23" s="299"/>
-      <c r="F23" s="299"/>
-      <c r="G23" s="299"/>
-      <c r="H23" s="299"/>
-      <c r="I23" s="300"/>
+      <c r="D23" s="294"/>
+      <c r="E23" s="294"/>
+      <c r="F23" s="294"/>
+      <c r="G23" s="294"/>
+      <c r="H23" s="294"/>
+      <c r="I23" s="295"/>
       <c r="M23" s="2"/>
     </row>
     <row r="24" spans="2:13" ht="18" customHeight="1">
       <c r="B24" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="294" t="s">
+      <c r="C24" s="296" t="s">
         <v>2268</v>
       </c>
-      <c r="D24" s="294"/>
-      <c r="E24" s="294"/>
-      <c r="F24" s="294"/>
-      <c r="G24" s="294"/>
-      <c r="H24" s="294"/>
-      <c r="I24" s="295"/>
+      <c r="D24" s="296"/>
+      <c r="E24" s="296"/>
+      <c r="F24" s="296"/>
+      <c r="G24" s="296"/>
+      <c r="H24" s="296"/>
+      <c r="I24" s="297"/>
       <c r="M24" s="2"/>
     </row>
     <row r="25" spans="2:13" ht="15.75" customHeight="1">
       <c r="B25" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="294" t="s">
+      <c r="C25" s="296" t="s">
         <v>2269</v>
       </c>
-      <c r="D25" s="294"/>
-      <c r="E25" s="294"/>
-      <c r="F25" s="294"/>
-      <c r="G25" s="294"/>
-      <c r="H25" s="294"/>
-      <c r="I25" s="295"/>
+      <c r="D25" s="296"/>
+      <c r="E25" s="296"/>
+      <c r="F25" s="296"/>
+      <c r="G25" s="296"/>
+      <c r="H25" s="296"/>
+      <c r="I25" s="297"/>
       <c r="J25" s="91"/>
       <c r="M25" s="2"/>
     </row>
@@ -66343,15 +66347,15 @@
       <c r="B26" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="294" t="s">
+      <c r="C26" s="296" t="s">
         <v>2270</v>
       </c>
-      <c r="D26" s="294"/>
-      <c r="E26" s="294"/>
-      <c r="F26" s="294"/>
-      <c r="G26" s="294"/>
-      <c r="H26" s="294"/>
-      <c r="I26" s="295"/>
+      <c r="D26" s="296"/>
+      <c r="E26" s="296"/>
+      <c r="F26" s="296"/>
+      <c r="G26" s="296"/>
+      <c r="H26" s="296"/>
+      <c r="I26" s="297"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -66361,28 +66365,28 @@
       <c r="B27" s="92" t="s">
         <v>2271</v>
       </c>
-      <c r="C27" s="301" t="s">
+      <c r="C27" s="298" t="s">
         <v>2272</v>
       </c>
-      <c r="D27" s="301"/>
-      <c r="E27" s="301"/>
-      <c r="F27" s="301"/>
-      <c r="G27" s="301"/>
-      <c r="H27" s="301"/>
-      <c r="I27" s="302"/>
+      <c r="D27" s="298"/>
+      <c r="E27" s="298"/>
+      <c r="F27" s="298"/>
+      <c r="G27" s="298"/>
+      <c r="H27" s="298"/>
+      <c r="I27" s="299"/>
       <c r="J27" s="25"/>
     </row>
     <row r="28" spans="2:13" ht="18" customHeight="1">
-      <c r="B28" s="282" t="s">
+      <c r="B28" s="300" t="s">
         <v>2273</v>
       </c>
-      <c r="C28" s="283"/>
-      <c r="D28" s="283"/>
-      <c r="E28" s="283"/>
-      <c r="F28" s="283"/>
-      <c r="G28" s="283"/>
-      <c r="H28" s="283"/>
-      <c r="I28" s="284"/>
+      <c r="C28" s="301"/>
+      <c r="D28" s="301"/>
+      <c r="E28" s="301"/>
+      <c r="F28" s="301"/>
+      <c r="G28" s="301"/>
+      <c r="H28" s="301"/>
+      <c r="I28" s="302"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -66446,15 +66450,15 @@
       <c r="B32" s="94" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="297" t="s">
+      <c r="C32" s="290" t="s">
         <v>2279</v>
       </c>
-      <c r="D32" s="297"/>
-      <c r="E32" s="297"/>
-      <c r="F32" s="297"/>
-      <c r="G32" s="297"/>
-      <c r="H32" s="297"/>
-      <c r="I32" s="298"/>
+      <c r="D32" s="290"/>
+      <c r="E32" s="290"/>
+      <c r="F32" s="290"/>
+      <c r="G32" s="290"/>
+      <c r="H32" s="290"/>
+      <c r="I32" s="291"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -66464,15 +66468,15 @@
       <c r="B33" s="94" t="s">
         <v>31</v>
       </c>
-      <c r="C33" s="297" t="s">
+      <c r="C33" s="290" t="s">
         <v>2280</v>
       </c>
-      <c r="D33" s="297"/>
-      <c r="E33" s="297"/>
-      <c r="F33" s="297"/>
-      <c r="G33" s="297"/>
-      <c r="H33" s="297"/>
-      <c r="I33" s="298"/>
+      <c r="D33" s="290"/>
+      <c r="E33" s="290"/>
+      <c r="F33" s="290"/>
+      <c r="G33" s="290"/>
+      <c r="H33" s="290"/>
+      <c r="I33" s="291"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -66482,15 +66486,15 @@
       <c r="B34" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="315" t="s">
+      <c r="C34" s="279" t="s">
         <v>2281</v>
       </c>
-      <c r="D34" s="315"/>
-      <c r="E34" s="315"/>
-      <c r="F34" s="315"/>
-      <c r="G34" s="315"/>
-      <c r="H34" s="315"/>
-      <c r="I34" s="316"/>
+      <c r="D34" s="279"/>
+      <c r="E34" s="279"/>
+      <c r="F34" s="279"/>
+      <c r="G34" s="279"/>
+      <c r="H34" s="279"/>
+      <c r="I34" s="280"/>
       <c r="J34" s="2"/>
       <c r="K34" s="90"/>
       <c r="L34" s="90"/>
@@ -66500,15 +66504,15 @@
       <c r="B35" s="96" t="s">
         <v>2282</v>
       </c>
-      <c r="C35" s="315" t="s">
+      <c r="C35" s="279" t="s">
         <v>2283</v>
       </c>
-      <c r="D35" s="315"/>
-      <c r="E35" s="315"/>
-      <c r="F35" s="315"/>
-      <c r="G35" s="315"/>
-      <c r="H35" s="315"/>
-      <c r="I35" s="316"/>
+      <c r="D35" s="279"/>
+      <c r="E35" s="279"/>
+      <c r="F35" s="279"/>
+      <c r="G35" s="279"/>
+      <c r="H35" s="279"/>
+      <c r="I35" s="280"/>
       <c r="J35" s="2"/>
       <c r="K35" s="90"/>
       <c r="L35" s="90"/>
@@ -66518,15 +66522,15 @@
       <c r="B36" s="97" t="s">
         <v>39</v>
       </c>
-      <c r="C36" s="315" t="s">
+      <c r="C36" s="279" t="s">
         <v>2284</v>
       </c>
-      <c r="D36" s="315"/>
-      <c r="E36" s="315"/>
-      <c r="F36" s="315"/>
-      <c r="G36" s="315"/>
-      <c r="H36" s="315"/>
-      <c r="I36" s="316"/>
+      <c r="D36" s="279"/>
+      <c r="E36" s="279"/>
+      <c r="F36" s="279"/>
+      <c r="G36" s="279"/>
+      <c r="H36" s="279"/>
+      <c r="I36" s="280"/>
       <c r="J36" s="2"/>
       <c r="K36" s="90"/>
       <c r="L36" s="90"/>
@@ -66536,15 +66540,15 @@
       <c r="B37" s="98" t="s">
         <v>40</v>
       </c>
-      <c r="C37" s="315" t="s">
+      <c r="C37" s="279" t="s">
         <v>2285</v>
       </c>
-      <c r="D37" s="315"/>
-      <c r="E37" s="315"/>
-      <c r="F37" s="315"/>
-      <c r="G37" s="315"/>
-      <c r="H37" s="315"/>
-      <c r="I37" s="316"/>
+      <c r="D37" s="279"/>
+      <c r="E37" s="279"/>
+      <c r="F37" s="279"/>
+      <c r="G37" s="279"/>
+      <c r="H37" s="279"/>
+      <c r="I37" s="280"/>
       <c r="J37" s="2"/>
       <c r="K37" s="90"/>
       <c r="L37" s="90"/>
@@ -66554,116 +66558,146 @@
       <c r="B38" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="C38" s="317" t="s">
+      <c r="C38" s="281" t="s">
         <v>2286</v>
       </c>
-      <c r="D38" s="318"/>
-      <c r="E38" s="318"/>
-      <c r="F38" s="318"/>
-      <c r="G38" s="318"/>
-      <c r="H38" s="318"/>
-      <c r="I38" s="319"/>
+      <c r="D38" s="282"/>
+      <c r="E38" s="282"/>
+      <c r="F38" s="282"/>
+      <c r="G38" s="282"/>
+      <c r="H38" s="282"/>
+      <c r="I38" s="283"/>
     </row>
     <row r="39" spans="2:13" ht="54.75" customHeight="1" thickBot="1">
       <c r="B39" s="99" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="317" t="s">
+      <c r="C39" s="281" t="s">
         <v>2287</v>
       </c>
-      <c r="D39" s="318"/>
-      <c r="E39" s="318"/>
-      <c r="F39" s="318"/>
-      <c r="G39" s="318"/>
-      <c r="H39" s="318"/>
-      <c r="I39" s="319"/>
+      <c r="D39" s="282"/>
+      <c r="E39" s="282"/>
+      <c r="F39" s="282"/>
+      <c r="G39" s="282"/>
+      <c r="H39" s="282"/>
+      <c r="I39" s="283"/>
     </row>
     <row r="40" spans="2:13" ht="40.5" customHeight="1" thickBot="1">
       <c r="B40" s="100" t="s">
         <v>2288</v>
       </c>
-      <c r="C40" s="320" t="s">
+      <c r="C40" s="284" t="s">
         <v>2289</v>
       </c>
-      <c r="D40" s="321"/>
-      <c r="E40" s="321"/>
-      <c r="F40" s="321"/>
-      <c r="G40" s="321"/>
-      <c r="H40" s="321"/>
-      <c r="I40" s="322"/>
+      <c r="D40" s="285"/>
+      <c r="E40" s="285"/>
+      <c r="F40" s="285"/>
+      <c r="G40" s="285"/>
+      <c r="H40" s="285"/>
+      <c r="I40" s="286"/>
     </row>
     <row r="41" spans="2:13" ht="40.5" customHeight="1" thickBot="1">
       <c r="B41" s="101" t="s">
         <v>2290</v>
       </c>
-      <c r="C41" s="323" t="s">
+      <c r="C41" s="287" t="s">
         <v>2291</v>
       </c>
-      <c r="D41" s="321"/>
-      <c r="E41" s="321"/>
-      <c r="F41" s="321"/>
-      <c r="G41" s="321"/>
-      <c r="H41" s="321"/>
-      <c r="I41" s="322"/>
+      <c r="D41" s="285"/>
+      <c r="E41" s="285"/>
+      <c r="F41" s="285"/>
+      <c r="G41" s="285"/>
+      <c r="H41" s="285"/>
+      <c r="I41" s="286"/>
     </row>
     <row r="42" spans="2:13" ht="40.5" customHeight="1" thickBot="1">
       <c r="B42" s="102" t="s">
         <v>2292</v>
       </c>
-      <c r="C42" s="324" t="s">
+      <c r="C42" s="288" t="s">
         <v>2293</v>
       </c>
-      <c r="D42" s="324"/>
-      <c r="E42" s="324"/>
-      <c r="F42" s="324"/>
-      <c r="G42" s="324"/>
-      <c r="H42" s="324"/>
-      <c r="I42" s="325"/>
+      <c r="D42" s="288"/>
+      <c r="E42" s="288"/>
+      <c r="F42" s="288"/>
+      <c r="G42" s="288"/>
+      <c r="H42" s="288"/>
+      <c r="I42" s="289"/>
     </row>
     <row r="43" spans="2:13" ht="43.5" customHeight="1" thickBot="1">
       <c r="B43" s="103" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="312" t="s">
+      <c r="C43" s="276" t="s">
         <v>2294</v>
       </c>
-      <c r="D43" s="313"/>
-      <c r="E43" s="313"/>
-      <c r="F43" s="313"/>
-      <c r="G43" s="313"/>
-      <c r="H43" s="313"/>
-      <c r="I43" s="314"/>
+      <c r="D43" s="277"/>
+      <c r="E43" s="277"/>
+      <c r="F43" s="277"/>
+      <c r="G43" s="277"/>
+      <c r="H43" s="277"/>
+      <c r="I43" s="278"/>
     </row>
     <row r="44" spans="2:13" ht="13.5" customHeight="1" thickBot="1">
       <c r="B44" s="103" t="s">
         <v>47</v>
       </c>
-      <c r="C44" s="312" t="s">
+      <c r="C44" s="276" t="s">
         <v>2295</v>
       </c>
-      <c r="D44" s="313"/>
-      <c r="E44" s="313"/>
-      <c r="F44" s="313"/>
-      <c r="G44" s="313"/>
-      <c r="H44" s="313"/>
-      <c r="I44" s="314"/>
+      <c r="D44" s="277"/>
+      <c r="E44" s="277"/>
+      <c r="F44" s="277"/>
+      <c r="G44" s="277"/>
+      <c r="H44" s="277"/>
+      <c r="I44" s="278"/>
     </row>
     <row r="45" spans="2:13" ht="32.25" customHeight="1" thickBot="1">
       <c r="B45" s="103" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="312" t="s">
+      <c r="C45" s="276" t="s">
         <v>2296</v>
       </c>
-      <c r="D45" s="313"/>
-      <c r="E45" s="313"/>
-      <c r="F45" s="313"/>
-      <c r="G45" s="313"/>
-      <c r="H45" s="313"/>
-      <c r="I45" s="314"/>
+      <c r="D45" s="277"/>
+      <c r="E45" s="277"/>
+      <c r="F45" s="277"/>
+      <c r="G45" s="277"/>
+      <c r="H45" s="277"/>
+      <c r="I45" s="278"/>
     </row>
   </sheetData>
   <mergeCells count="42">
+    <mergeCell ref="C9:I9"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C8:I8"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="D14:H14"/>
+    <mergeCell ref="D15:H15"/>
+    <mergeCell ref="D16:H16"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="C20:I20"/>
+    <mergeCell ref="C21:I21"/>
+    <mergeCell ref="C33:I33"/>
+    <mergeCell ref="C22:I22"/>
+    <mergeCell ref="C23:I23"/>
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="C25:I25"/>
+    <mergeCell ref="C26:I26"/>
+    <mergeCell ref="C27:I27"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="C29:I29"/>
+    <mergeCell ref="C30:I30"/>
+    <mergeCell ref="C31:I31"/>
+    <mergeCell ref="C32:I32"/>
     <mergeCell ref="C45:I45"/>
     <mergeCell ref="C34:I34"/>
     <mergeCell ref="C35:I35"/>
@@ -66676,36 +66710,6 @@
     <mergeCell ref="C42:I42"/>
     <mergeCell ref="C43:I43"/>
     <mergeCell ref="C44:I44"/>
-    <mergeCell ref="C33:I33"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="C23:I23"/>
-    <mergeCell ref="C24:I24"/>
-    <mergeCell ref="C25:I25"/>
-    <mergeCell ref="C26:I26"/>
-    <mergeCell ref="C27:I27"/>
-    <mergeCell ref="B28:I28"/>
-    <mergeCell ref="C29:I29"/>
-    <mergeCell ref="C30:I30"/>
-    <mergeCell ref="C31:I31"/>
-    <mergeCell ref="C32:I32"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="D10:H10"/>
-    <mergeCell ref="D11:H11"/>
-    <mergeCell ref="D12:H12"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="D14:H14"/>
-    <mergeCell ref="D15:H15"/>
-    <mergeCell ref="D16:H16"/>
-    <mergeCell ref="D17:H17"/>
-    <mergeCell ref="D18:H18"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C9:I9"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B6:I6"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C8:I8"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H1" location="Ballot!A1" display="Ballot!A1"/>
@@ -68445,7 +68449,7 @@
       <c r="A3" s="330" t="s">
         <v>2305</v>
       </c>
-      <c r="B3" s="333" t="s">
+      <c r="B3" s="332" t="s">
         <v>2306</v>
       </c>
       <c r="C3" s="124" t="s">
@@ -68460,7 +68464,7 @@
     </row>
     <row r="4" spans="1:5" ht="28.5" customHeight="1">
       <c r="A4" s="331"/>
-      <c r="B4" s="334"/>
+      <c r="B4" s="333"/>
       <c r="C4" s="124" t="s">
         <v>2310</v>
       </c>
@@ -68473,7 +68477,7 @@
     </row>
     <row r="5" spans="1:5" ht="28.5" customHeight="1">
       <c r="A5" s="331"/>
-      <c r="B5" s="334"/>
+      <c r="B5" s="333"/>
       <c r="C5" s="124" t="s">
         <v>2313</v>
       </c>
@@ -68486,7 +68490,7 @@
     </row>
     <row r="6" spans="1:5" ht="14.25" customHeight="1">
       <c r="A6" s="331"/>
-      <c r="B6" s="334"/>
+      <c r="B6" s="333"/>
       <c r="C6" s="124" t="s">
         <v>2315</v>
       </c>
@@ -68499,7 +68503,7 @@
     </row>
     <row r="7" spans="1:5" ht="14.25" customHeight="1">
       <c r="A7" s="331"/>
-      <c r="B7" s="334"/>
+      <c r="B7" s="333"/>
       <c r="C7" s="124" t="s">
         <v>2254</v>
       </c>
@@ -68512,7 +68516,7 @@
     </row>
     <row r="8" spans="1:5" ht="14.25" customHeight="1">
       <c r="A8" s="331"/>
-      <c r="B8" s="334"/>
+      <c r="B8" s="333"/>
       <c r="C8" s="124" t="s">
         <v>2318</v>
       </c>
@@ -68525,7 +68529,7 @@
     </row>
     <row r="9" spans="1:5" ht="28.5" customHeight="1">
       <c r="A9" s="331"/>
-      <c r="B9" s="334"/>
+      <c r="B9" s="333"/>
       <c r="C9" s="124" t="s">
         <v>2321</v>
       </c>
@@ -68538,7 +68542,7 @@
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1">
       <c r="A10" s="331"/>
-      <c r="B10" s="334"/>
+      <c r="B10" s="333"/>
       <c r="C10" s="124" t="s">
         <v>2323</v>
       </c>
@@ -68550,8 +68554,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A11" s="332"/>
-      <c r="B11" s="335"/>
+      <c r="A11" s="338"/>
+      <c r="B11" s="334"/>
       <c r="C11" s="124" t="s">
         <v>2326</v>
       </c>
@@ -68718,7 +68722,7 @@
       <c r="A26" s="330" t="s">
         <v>2351</v>
       </c>
-      <c r="B26" s="333" t="s">
+      <c r="B26" s="332" t="s">
         <v>2352</v>
       </c>
       <c r="C26" s="124" t="s">
@@ -68733,7 +68737,7 @@
     </row>
     <row r="27" spans="1:5" ht="14.25" customHeight="1">
       <c r="A27" s="331"/>
-      <c r="B27" s="334"/>
+      <c r="B27" s="333"/>
       <c r="C27" s="131" t="s">
         <v>2355</v>
       </c>
@@ -68746,7 +68750,7 @@
     </row>
     <row r="28" spans="1:5" ht="14.25" customHeight="1">
       <c r="A28" s="331"/>
-      <c r="B28" s="334"/>
+      <c r="B28" s="333"/>
       <c r="C28" s="131" t="s">
         <v>2357</v>
       </c>
@@ -68759,7 +68763,7 @@
     </row>
     <row r="29" spans="1:5" ht="14.25" customHeight="1">
       <c r="A29" s="331"/>
-      <c r="B29" s="334"/>
+      <c r="B29" s="333"/>
       <c r="C29" s="131" t="s">
         <v>2359</v>
       </c>
@@ -68772,7 +68776,7 @@
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1">
       <c r="A30" s="331"/>
-      <c r="B30" s="334"/>
+      <c r="B30" s="333"/>
       <c r="C30" s="131" t="s">
         <v>2361</v>
       </c>
@@ -68958,7 +68962,7 @@
       <c r="A46" s="330" t="s">
         <v>638</v>
       </c>
-      <c r="B46" s="336" t="s">
+      <c r="B46" s="335" t="s">
         <v>2386</v>
       </c>
       <c r="C46" s="124" t="s">
@@ -68973,7 +68977,7 @@
     </row>
     <row r="47" spans="1:5" ht="14.25" customHeight="1">
       <c r="A47" s="331"/>
-      <c r="B47" s="337"/>
+      <c r="B47" s="336"/>
       <c r="C47" s="124" t="s">
         <v>2388</v>
       </c>
@@ -68986,7 +68990,7 @@
     </row>
     <row r="48" spans="1:5" ht="14.25" customHeight="1">
       <c r="A48" s="331"/>
-      <c r="B48" s="338"/>
+      <c r="B48" s="337"/>
       <c r="C48" s="124" t="s">
         <v>2390</v>
       </c>
@@ -69050,7 +69054,7 @@
       <c r="A54" s="330" t="s">
         <v>2398</v>
       </c>
-      <c r="B54" s="333" t="s">
+      <c r="B54" s="332" t="s">
         <v>2399</v>
       </c>
       <c r="C54" s="124" t="s">
@@ -69065,7 +69069,7 @@
     </row>
     <row r="55" spans="1:5" ht="14.25" customHeight="1">
       <c r="A55" s="331"/>
-      <c r="B55" s="334"/>
+      <c r="B55" s="333"/>
       <c r="C55" s="124" t="s">
         <v>2402</v>
       </c>
@@ -69078,7 +69082,7 @@
     </row>
     <row r="56" spans="1:5" ht="14.25" customHeight="1">
       <c r="A56" s="331"/>
-      <c r="B56" s="335"/>
+      <c r="B56" s="334"/>
       <c r="C56" s="124" t="s">
         <v>2404</v>
       </c>
@@ -69280,6 +69284,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A3:A11"/>
+    <mergeCell ref="B3:B11"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="A23:A24"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="B26:B30"/>
+    <mergeCell ref="A34:A43"/>
+    <mergeCell ref="B34:B43"/>
+    <mergeCell ref="A46:A48"/>
+    <mergeCell ref="B46:B48"/>
     <mergeCell ref="A66:A67"/>
     <mergeCell ref="B66:B67"/>
     <mergeCell ref="A69:A70"/>
@@ -69290,18 +69306,6 @@
     <mergeCell ref="B58:B59"/>
     <mergeCell ref="A61:A62"/>
     <mergeCell ref="B61:B62"/>
-    <mergeCell ref="A26:A30"/>
-    <mergeCell ref="B26:B30"/>
-    <mergeCell ref="A34:A43"/>
-    <mergeCell ref="B34:B43"/>
-    <mergeCell ref="A46:A48"/>
-    <mergeCell ref="B46:B48"/>
-    <mergeCell ref="A3:A11"/>
-    <mergeCell ref="B3:B11"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="B23:B24"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>